<commit_message>
Fixes invalid MODS language authority
</commit_message>
<xml_diff>
--- a/spec/fixtures/Heckrotte_ChartsOfCoastSurvey.xlsx
+++ b/spec/fixtures/Heckrotte_ChartsOfCoastSurvey.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sdoljack/Documents/GitHub/modsulator/spec/fixtures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arcadia\Box Sync\Projects\Digital collections\modsulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16140" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Charts of the Coast Survey" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="IA1" authorId="0">
+    <comment ref="IA1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2989" uniqueCount="686">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2989" uniqueCount="689">
   <si>
     <t>Identification</t>
   </si>
@@ -2104,6 +2104,15 @@
   </si>
   <si>
     <t>inferred</t>
+  </si>
+  <si>
+    <t>iso639-2b</t>
+  </si>
+  <si>
+    <t>http://id.loc.gov/vocabulary/iso639-2</t>
+  </si>
+  <si>
+    <t>http://id.loc.gov/vocabulary/iso639-2/eng</t>
   </si>
 </sst>
 </file>
@@ -2113,7 +2122,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="28">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2563,16 +2572,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2582,6 +2591,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2908,20 +2920,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:JR1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="IS19" sqref="IS19"/>
+    <sheetView tabSelected="1" topLeftCell="BX1" workbookViewId="0">
+      <selection activeCell="CE5" sqref="CE5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
     <col min="4" max="4" width="44" customWidth="1"/>
-    <col min="8" max="8" width="22.6640625" customWidth="1"/>
-    <col min="88" max="88" width="27.5" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" customWidth="1"/>
+    <col min="88" max="88" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:278" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="105" t="s">
+    <row r="1" spans="1:278">
+      <c r="A1" s="110" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="108"/>
@@ -2995,10 +3007,10 @@
       <c r="BD1" s="5"/>
       <c r="BE1" s="5"/>
       <c r="BF1" s="5"/>
-      <c r="BG1" s="105" t="s">
+      <c r="BG1" s="110" t="s">
         <v>4</v>
       </c>
-      <c r="BH1" s="106"/>
+      <c r="BH1" s="112"/>
       <c r="BI1" s="4" t="s">
         <v>5</v>
       </c>
@@ -3031,14 +3043,14 @@
       <c r="CB1" s="2"/>
       <c r="CC1" s="2"/>
       <c r="CD1" s="2"/>
-      <c r="CE1" s="107" t="s">
+      <c r="CE1" s="111" t="s">
         <v>11</v>
       </c>
       <c r="CF1" s="108"/>
       <c r="CG1" s="2"/>
       <c r="CH1" s="2"/>
       <c r="CI1" s="2"/>
-      <c r="CJ1" s="105" t="s">
+      <c r="CJ1" s="110" t="s">
         <v>12</v>
       </c>
       <c r="CK1" s="108"/>
@@ -3240,12 +3252,12 @@
       <c r="HG1" s="2"/>
       <c r="HH1" s="2"/>
       <c r="HI1" s="2"/>
-      <c r="HJ1" s="107" t="s">
+      <c r="HJ1" s="111" t="s">
         <v>24</v>
       </c>
       <c r="HK1" s="108"/>
       <c r="HL1" s="2"/>
-      <c r="HM1" s="110" t="s">
+      <c r="HM1" s="107" t="s">
         <v>25</v>
       </c>
       <c r="HN1" s="108"/>
@@ -3318,7 +3330,7 @@
       <c r="JQ1" s="20"/>
       <c r="JR1" s="20"/>
     </row>
-    <row r="2" spans="1:278" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:278">
       <c r="A2" s="10" t="s">
         <v>32</v>
       </c>
@@ -4094,7 +4106,7 @@
       <c r="JQ2" s="29"/>
       <c r="JR2" s="29"/>
     </row>
-    <row r="3" spans="1:278" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:278">
       <c r="A3" s="30" t="s">
         <v>323</v>
       </c>
@@ -4289,7 +4301,7 @@
       <c r="BZ3" s="33" t="s">
         <v>344</v>
       </c>
-      <c r="CA3" s="111" t="s">
+      <c r="CA3" s="105" t="s">
         <v>682</v>
       </c>
       <c r="CB3" s="33" t="s">
@@ -4308,13 +4320,13 @@
         <v>346</v>
       </c>
       <c r="CG3" s="33" t="s">
-        <v>163</v>
+        <v>686</v>
       </c>
       <c r="CH3" s="43" t="s">
-        <v>164</v>
+        <v>687</v>
       </c>
       <c r="CI3" s="34" t="s">
-        <v>180</v>
+        <v>688</v>
       </c>
       <c r="CJ3" s="48" t="s">
         <v>165</v>
@@ -4605,7 +4617,7 @@
       <c r="IB3" s="42" t="s">
         <v>160</v>
       </c>
-      <c r="IC3" s="112" t="s">
+      <c r="IC3" s="106" t="s">
         <v>685</v>
       </c>
       <c r="ID3" s="59" t="s">
@@ -4614,7 +4626,7 @@
       <c r="IE3" s="48" t="s">
         <v>344</v>
       </c>
-      <c r="IF3" s="111" t="s">
+      <c r="IF3" s="105" t="s">
         <v>682</v>
       </c>
       <c r="IG3" s="48" t="s">
@@ -4672,7 +4684,7 @@
       <c r="JQ3" s="39"/>
       <c r="JR3" s="32"/>
     </row>
-    <row r="4" spans="1:278" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:278">
       <c r="A4" s="30" t="s">
         <v>367</v>
       </c>
@@ -4877,7 +4889,7 @@
       <c r="BZ4" s="33" t="s">
         <v>344</v>
       </c>
-      <c r="CA4" s="111" t="s">
+      <c r="CA4" s="105" t="s">
         <v>682</v>
       </c>
       <c r="CB4" s="33" t="s">
@@ -4895,14 +4907,14 @@
       <c r="CF4" s="33" t="s">
         <v>346</v>
       </c>
-      <c r="CG4" s="33" t="s">
-        <v>163</v>
+      <c r="CG4" s="73" t="s">
+        <v>686</v>
       </c>
       <c r="CH4" s="43" t="s">
-        <v>164</v>
+        <v>687</v>
       </c>
       <c r="CI4" s="34" t="s">
-        <v>180</v>
+        <v>688</v>
       </c>
       <c r="CJ4" s="48" t="s">
         <v>165</v>
@@ -5287,7 +5299,7 @@
       <c r="IB4" s="42" t="s">
         <v>160</v>
       </c>
-      <c r="IC4" s="112" t="s">
+      <c r="IC4" s="106" t="s">
         <v>685</v>
       </c>
       <c r="ID4" s="59" t="s">
@@ -5296,7 +5308,7 @@
       <c r="IE4" s="48" t="s">
         <v>344</v>
       </c>
-      <c r="IF4" s="111" t="s">
+      <c r="IF4" s="105" t="s">
         <v>682</v>
       </c>
       <c r="IG4" s="48" t="s">
@@ -5324,7 +5336,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="5" spans="1:278" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:278">
       <c r="A5" s="30" t="s">
         <v>401</v>
       </c>
@@ -5529,7 +5541,7 @@
       <c r="BZ5" s="33" t="s">
         <v>344</v>
       </c>
-      <c r="CA5" s="111" t="s">
+      <c r="CA5" s="105" t="s">
         <v>682</v>
       </c>
       <c r="CB5" s="33" t="s">
@@ -5547,14 +5559,14 @@
       <c r="CF5" s="33" t="s">
         <v>346</v>
       </c>
-      <c r="CG5" s="33" t="s">
-        <v>163</v>
+      <c r="CG5" s="73" t="s">
+        <v>686</v>
       </c>
       <c r="CH5" s="43" t="s">
-        <v>164</v>
+        <v>687</v>
       </c>
       <c r="CI5" s="34" t="s">
-        <v>180</v>
+        <v>688</v>
       </c>
       <c r="CJ5" s="48" t="s">
         <v>165</v>
@@ -5843,7 +5855,7 @@
       <c r="IB5" s="42" t="s">
         <v>160</v>
       </c>
-      <c r="IC5" s="112" t="s">
+      <c r="IC5" s="106" t="s">
         <v>685</v>
       </c>
       <c r="ID5" s="59" t="s">
@@ -5852,7 +5864,7 @@
       <c r="IE5" s="48" t="s">
         <v>344</v>
       </c>
-      <c r="IF5" s="111" t="s">
+      <c r="IF5" s="105" t="s">
         <v>682</v>
       </c>
       <c r="IG5" s="48" t="s">
@@ -5880,7 +5892,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="6" spans="1:278" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:278">
       <c r="A6" s="30" t="s">
         <v>419</v>
       </c>
@@ -6095,7 +6107,7 @@
       <c r="BZ6" s="33" t="s">
         <v>344</v>
       </c>
-      <c r="CA6" s="111" t="s">
+      <c r="CA6" s="105" t="s">
         <v>682</v>
       </c>
       <c r="CB6" s="33" t="s">
@@ -6113,14 +6125,14 @@
       <c r="CF6" s="33" t="s">
         <v>346</v>
       </c>
-      <c r="CG6" s="33" t="s">
-        <v>163</v>
+      <c r="CG6" s="73" t="s">
+        <v>686</v>
       </c>
       <c r="CH6" s="43" t="s">
-        <v>164</v>
+        <v>687</v>
       </c>
       <c r="CI6" s="34" t="s">
-        <v>180</v>
+        <v>688</v>
       </c>
       <c r="CJ6" s="48" t="s">
         <v>165</v>
@@ -6423,7 +6435,7 @@
       <c r="IB6" s="42" t="s">
         <v>160</v>
       </c>
-      <c r="IC6" s="112" t="s">
+      <c r="IC6" s="106" t="s">
         <v>685</v>
       </c>
       <c r="ID6" s="60" t="s">
@@ -6432,7 +6444,7 @@
       <c r="IE6" s="48" t="s">
         <v>344</v>
       </c>
-      <c r="IF6" s="111" t="s">
+      <c r="IF6" s="105" t="s">
         <v>682</v>
       </c>
       <c r="IG6" s="48" t="s">
@@ -6460,7 +6472,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="7" spans="1:278" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:278">
       <c r="A7" s="30" t="s">
         <v>435</v>
       </c>
@@ -6641,7 +6653,7 @@
       <c r="BZ7" s="33" t="s">
         <v>344</v>
       </c>
-      <c r="CA7" s="111" t="s">
+      <c r="CA7" s="105" t="s">
         <v>682</v>
       </c>
       <c r="CB7" s="33" t="s">
@@ -6659,14 +6671,14 @@
       <c r="CF7" s="33" t="s">
         <v>346</v>
       </c>
-      <c r="CG7" s="33" t="s">
-        <v>163</v>
+      <c r="CG7" s="73" t="s">
+        <v>686</v>
       </c>
       <c r="CH7" s="43" t="s">
-        <v>164</v>
+        <v>687</v>
       </c>
       <c r="CI7" s="34" t="s">
-        <v>180</v>
+        <v>688</v>
       </c>
       <c r="CJ7" s="48" t="s">
         <v>165</v>
@@ -7051,7 +7063,7 @@
       <c r="IB7" s="42" t="s">
         <v>160</v>
       </c>
-      <c r="IC7" s="112" t="s">
+      <c r="IC7" s="106" t="s">
         <v>685</v>
       </c>
       <c r="ID7" s="59" t="s">
@@ -7060,7 +7072,7 @@
       <c r="IE7" s="48" t="s">
         <v>344</v>
       </c>
-      <c r="IF7" s="111" t="s">
+      <c r="IF7" s="105" t="s">
         <v>682</v>
       </c>
       <c r="IG7" s="48" t="s">
@@ -7088,7 +7100,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="8" spans="1:278" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:278">
       <c r="A8" s="30" t="s">
         <v>461</v>
       </c>
@@ -7289,7 +7301,7 @@
       <c r="BZ8" s="33" t="s">
         <v>344</v>
       </c>
-      <c r="CA8" s="111" t="s">
+      <c r="CA8" s="105" t="s">
         <v>682</v>
       </c>
       <c r="CB8" s="33" t="s">
@@ -7307,14 +7319,14 @@
       <c r="CF8" s="33" t="s">
         <v>346</v>
       </c>
-      <c r="CG8" s="33" t="s">
-        <v>163</v>
+      <c r="CG8" s="73" t="s">
+        <v>686</v>
       </c>
       <c r="CH8" s="43" t="s">
-        <v>164</v>
+        <v>687</v>
       </c>
       <c r="CI8" s="34" t="s">
-        <v>180</v>
+        <v>688</v>
       </c>
       <c r="CJ8" s="48" t="s">
         <v>165</v>
@@ -7607,7 +7619,7 @@
       <c r="IB8" s="42" t="s">
         <v>160</v>
       </c>
-      <c r="IC8" s="112" t="s">
+      <c r="IC8" s="106" t="s">
         <v>685</v>
       </c>
       <c r="ID8" s="60" t="s">
@@ -7616,7 +7628,7 @@
       <c r="IE8" s="48" t="s">
         <v>344</v>
       </c>
-      <c r="IF8" s="111" t="s">
+      <c r="IF8" s="105" t="s">
         <v>682</v>
       </c>
       <c r="IG8" s="48" t="s">
@@ -7644,7 +7656,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="9" spans="1:278" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:278">
       <c r="A9" s="92" t="s">
         <v>488</v>
       </c>
@@ -7845,7 +7857,7 @@
       <c r="BZ9" s="33" t="s">
         <v>344</v>
       </c>
-      <c r="CA9" s="111" t="s">
+      <c r="CA9" s="105" t="s">
         <v>682</v>
       </c>
       <c r="CB9" s="33" t="s">
@@ -7863,14 +7875,14 @@
       <c r="CF9" s="33" t="s">
         <v>346</v>
       </c>
-      <c r="CG9" s="33" t="s">
-        <v>163</v>
+      <c r="CG9" s="73" t="s">
+        <v>686</v>
       </c>
       <c r="CH9" s="43" t="s">
-        <v>164</v>
+        <v>687</v>
       </c>
       <c r="CI9" s="34" t="s">
-        <v>180</v>
+        <v>688</v>
       </c>
       <c r="CJ9" s="48" t="s">
         <v>165</v>
@@ -8100,7 +8112,7 @@
       <c r="IB9" s="42" t="s">
         <v>160</v>
       </c>
-      <c r="IC9" s="112" t="s">
+      <c r="IC9" s="106" t="s">
         <v>685</v>
       </c>
       <c r="ID9" s="60" t="s">
@@ -8109,7 +8121,7 @@
       <c r="IE9" s="48" t="s">
         <v>344</v>
       </c>
-      <c r="IF9" s="111" t="s">
+      <c r="IF9" s="105" t="s">
         <v>682</v>
       </c>
       <c r="IG9" s="48" t="s">
@@ -8137,7 +8149,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="10" spans="1:278" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:278">
       <c r="A10" s="92" t="s">
         <v>505</v>
       </c>
@@ -8336,7 +8348,7 @@
       <c r="BZ10" s="33" t="s">
         <v>344</v>
       </c>
-      <c r="CA10" s="111" t="s">
+      <c r="CA10" s="105" t="s">
         <v>682</v>
       </c>
       <c r="CB10" s="33" t="s">
@@ -8354,14 +8366,14 @@
       <c r="CF10" s="33" t="s">
         <v>346</v>
       </c>
-      <c r="CG10" s="33" t="s">
-        <v>163</v>
+      <c r="CG10" s="73" t="s">
+        <v>686</v>
       </c>
       <c r="CH10" s="43" t="s">
-        <v>164</v>
+        <v>687</v>
       </c>
       <c r="CI10" s="34" t="s">
-        <v>180</v>
+        <v>688</v>
       </c>
       <c r="CJ10" s="48" t="s">
         <v>165</v>
@@ -8661,7 +8673,7 @@
       <c r="IB10" s="42" t="s">
         <v>160</v>
       </c>
-      <c r="IC10" s="112" t="s">
+      <c r="IC10" s="106" t="s">
         <v>685</v>
       </c>
       <c r="ID10" s="59" t="s">
@@ -8670,7 +8682,7 @@
       <c r="IE10" s="48" t="s">
         <v>344</v>
       </c>
-      <c r="IF10" s="111" t="s">
+      <c r="IF10" s="105" t="s">
         <v>682</v>
       </c>
       <c r="IG10" s="48" t="s">
@@ -8698,7 +8710,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="11" spans="1:278" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:278">
       <c r="A11" s="92" t="s">
         <v>527</v>
       </c>
@@ -8897,7 +8909,7 @@
       <c r="BZ11" s="33" t="s">
         <v>344</v>
       </c>
-      <c r="CA11" s="111" t="s">
+      <c r="CA11" s="105" t="s">
         <v>682</v>
       </c>
       <c r="CB11" s="33" t="s">
@@ -8915,14 +8927,14 @@
       <c r="CF11" s="33" t="s">
         <v>346</v>
       </c>
-      <c r="CG11" s="33" t="s">
-        <v>163</v>
+      <c r="CG11" s="73" t="s">
+        <v>686</v>
       </c>
       <c r="CH11" s="43" t="s">
-        <v>164</v>
+        <v>687</v>
       </c>
       <c r="CI11" s="34" t="s">
-        <v>180</v>
+        <v>688</v>
       </c>
       <c r="CJ11" s="48" t="s">
         <v>165</v>
@@ -9335,7 +9347,7 @@
       <c r="IB11" s="42" t="s">
         <v>160</v>
       </c>
-      <c r="IC11" s="112" t="s">
+      <c r="IC11" s="106" t="s">
         <v>685</v>
       </c>
       <c r="ID11" s="59" t="s">
@@ -9344,7 +9356,7 @@
       <c r="IE11" s="48" t="s">
         <v>344</v>
       </c>
-      <c r="IF11" s="111" t="s">
+      <c r="IF11" s="105" t="s">
         <v>682</v>
       </c>
       <c r="IG11" s="48" t="s">
@@ -9372,7 +9384,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="12" spans="1:278" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:278">
       <c r="A12" s="92" t="s">
         <v>555</v>
       </c>
@@ -9557,7 +9569,7 @@
       <c r="BZ12" s="33" t="s">
         <v>344</v>
       </c>
-      <c r="CA12" s="111" t="s">
+      <c r="CA12" s="105" t="s">
         <v>682</v>
       </c>
       <c r="CB12" s="33" t="s">
@@ -9575,14 +9587,14 @@
       <c r="CF12" s="33" t="s">
         <v>346</v>
       </c>
-      <c r="CG12" s="33" t="s">
-        <v>163</v>
+      <c r="CG12" s="73" t="s">
+        <v>686</v>
       </c>
       <c r="CH12" s="43" t="s">
-        <v>164</v>
+        <v>687</v>
       </c>
       <c r="CI12" s="34" t="s">
-        <v>180</v>
+        <v>688</v>
       </c>
       <c r="CJ12" s="48" t="s">
         <v>165</v>
@@ -9928,7 +9940,7 @@
       <c r="IB12" s="42" t="s">
         <v>160</v>
       </c>
-      <c r="IC12" s="112" t="s">
+      <c r="IC12" s="106" t="s">
         <v>685</v>
       </c>
       <c r="ID12" s="59" t="s">
@@ -9937,7 +9949,7 @@
       <c r="IE12" s="48" t="s">
         <v>344</v>
       </c>
-      <c r="IF12" s="111" t="s">
+      <c r="IF12" s="105" t="s">
         <v>682</v>
       </c>
       <c r="IG12" s="48" t="s">
@@ -9965,7 +9977,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="13" spans="1:278" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:278">
       <c r="A13" s="92" t="s">
         <v>577</v>
       </c>
@@ -10164,7 +10176,7 @@
       <c r="BZ13" s="33" t="s">
         <v>344</v>
       </c>
-      <c r="CA13" s="111" t="s">
+      <c r="CA13" s="105" t="s">
         <v>682</v>
       </c>
       <c r="CB13" s="33" t="s">
@@ -10182,14 +10194,14 @@
       <c r="CF13" s="33" t="s">
         <v>346</v>
       </c>
-      <c r="CG13" s="33" t="s">
-        <v>163</v>
+      <c r="CG13" s="73" t="s">
+        <v>686</v>
       </c>
       <c r="CH13" s="43" t="s">
-        <v>164</v>
+        <v>687</v>
       </c>
       <c r="CI13" s="34" t="s">
-        <v>180</v>
+        <v>688</v>
       </c>
       <c r="CJ13" s="48" t="s">
         <v>165</v>
@@ -10440,7 +10452,7 @@
       <c r="IB13" s="42" t="s">
         <v>160</v>
       </c>
-      <c r="IC13" s="112" t="s">
+      <c r="IC13" s="106" t="s">
         <v>685</v>
       </c>
       <c r="ID13" s="59" t="s">
@@ -10449,7 +10461,7 @@
       <c r="IE13" s="48" t="s">
         <v>344</v>
       </c>
-      <c r="IF13" s="111" t="s">
+      <c r="IF13" s="105" t="s">
         <v>682</v>
       </c>
       <c r="IG13" s="48" t="s">
@@ -10477,7 +10489,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="14" spans="1:278" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:278">
       <c r="A14" s="92" t="s">
         <v>595</v>
       </c>
@@ -10678,7 +10690,7 @@
       <c r="BZ14" s="33" t="s">
         <v>344</v>
       </c>
-      <c r="CA14" s="111" t="s">
+      <c r="CA14" s="105" t="s">
         <v>682</v>
       </c>
       <c r="CB14" s="33" t="s">
@@ -10696,14 +10708,14 @@
       <c r="CF14" s="33" t="s">
         <v>346</v>
       </c>
-      <c r="CG14" s="33" t="s">
-        <v>163</v>
+      <c r="CG14" s="73" t="s">
+        <v>686</v>
       </c>
       <c r="CH14" s="43" t="s">
-        <v>164</v>
+        <v>687</v>
       </c>
       <c r="CI14" s="34" t="s">
-        <v>180</v>
+        <v>688</v>
       </c>
       <c r="CJ14" s="48" t="s">
         <v>165</v>
@@ -10874,7 +10886,7 @@
       <c r="IB14" s="42" t="s">
         <v>160</v>
       </c>
-      <c r="IC14" s="112" t="s">
+      <c r="IC14" s="106" t="s">
         <v>685</v>
       </c>
       <c r="ID14" s="59" t="s">
@@ -10883,7 +10895,7 @@
       <c r="IE14" s="48" t="s">
         <v>344</v>
       </c>
-      <c r="IF14" s="111" t="s">
+      <c r="IF14" s="105" t="s">
         <v>682</v>
       </c>
       <c r="IG14" s="48" t="s">
@@ -10911,7 +10923,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="15" spans="1:278" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:278">
       <c r="A15" s="92" t="s">
         <v>616</v>
       </c>
@@ -11120,7 +11132,7 @@
       <c r="BZ15" s="33" t="s">
         <v>344</v>
       </c>
-      <c r="CA15" s="111" t="s">
+      <c r="CA15" s="105" t="s">
         <v>682</v>
       </c>
       <c r="CB15" s="33" t="s">
@@ -11138,14 +11150,14 @@
       <c r="CF15" s="33" t="s">
         <v>346</v>
       </c>
-      <c r="CG15" s="33" t="s">
-        <v>163</v>
+      <c r="CG15" s="73" t="s">
+        <v>686</v>
       </c>
       <c r="CH15" s="43" t="s">
-        <v>164</v>
+        <v>687</v>
       </c>
       <c r="CI15" s="34" t="s">
-        <v>180</v>
+        <v>688</v>
       </c>
       <c r="CJ15" s="48" t="s">
         <v>165</v>
@@ -11556,7 +11568,7 @@
       <c r="IB15" s="42" t="s">
         <v>160</v>
       </c>
-      <c r="IC15" s="112" t="s">
+      <c r="IC15" s="106" t="s">
         <v>685</v>
       </c>
       <c r="ID15" s="59" t="s">
@@ -11565,7 +11577,7 @@
       <c r="IE15" s="48" t="s">
         <v>344</v>
       </c>
-      <c r="IF15" s="111" t="s">
+      <c r="IF15" s="105" t="s">
         <v>682</v>
       </c>
       <c r="IG15" s="48" t="s">
@@ -11593,7 +11605,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="16" spans="1:278" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:278">
       <c r="A16" s="92" t="s">
         <v>646</v>
       </c>
@@ -11794,7 +11806,7 @@
       <c r="BZ16" s="33" t="s">
         <v>344</v>
       </c>
-      <c r="CA16" s="111" t="s">
+      <c r="CA16" s="105" t="s">
         <v>682</v>
       </c>
       <c r="CB16" s="33" t="s">
@@ -11812,14 +11824,14 @@
       <c r="CF16" s="33" t="s">
         <v>346</v>
       </c>
-      <c r="CG16" s="33" t="s">
-        <v>163</v>
+      <c r="CG16" s="73" t="s">
+        <v>686</v>
       </c>
       <c r="CH16" s="43" t="s">
-        <v>164</v>
+        <v>687</v>
       </c>
       <c r="CI16" s="34" t="s">
-        <v>180</v>
+        <v>688</v>
       </c>
       <c r="CJ16" s="48" t="s">
         <v>165</v>
@@ -12179,7 +12191,7 @@
       <c r="IB16" s="42" t="s">
         <v>160</v>
       </c>
-      <c r="IC16" s="112" t="s">
+      <c r="IC16" s="106" t="s">
         <v>685</v>
       </c>
       <c r="ID16" s="59" t="s">
@@ -12188,7 +12200,7 @@
       <c r="IE16" s="48" t="s">
         <v>344</v>
       </c>
-      <c r="IF16" s="111" t="s">
+      <c r="IF16" s="105" t="s">
         <v>682</v>
       </c>
       <c r="IG16" s="48" t="s">
@@ -12216,7 +12228,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="17" spans="1:248" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:248">
       <c r="A17" s="92" t="s">
         <v>665</v>
       </c>
@@ -12416,7 +12428,7 @@
       <c r="BZ17" s="33" t="s">
         <v>344</v>
       </c>
-      <c r="CA17" s="111" t="s">
+      <c r="CA17" s="105" t="s">
         <v>682</v>
       </c>
       <c r="CB17" s="33" t="s">
@@ -12434,14 +12446,14 @@
       <c r="CF17" s="33" t="s">
         <v>346</v>
       </c>
-      <c r="CG17" s="33" t="s">
-        <v>163</v>
+      <c r="CG17" s="73" t="s">
+        <v>686</v>
       </c>
       <c r="CH17" s="43" t="s">
-        <v>164</v>
+        <v>687</v>
       </c>
       <c r="CI17" s="34" t="s">
-        <v>180</v>
+        <v>688</v>
       </c>
       <c r="CJ17" s="48" t="s">
         <v>165</v>
@@ -12736,7 +12748,7 @@
       <c r="IB17" s="42" t="s">
         <v>160</v>
       </c>
-      <c r="IC17" s="112" t="s">
+      <c r="IC17" s="106" t="s">
         <v>685</v>
       </c>
       <c r="ID17" s="59" t="s">
@@ -12745,7 +12757,7 @@
       <c r="IE17" s="48" t="s">
         <v>344</v>
       </c>
-      <c r="IF17" s="111" t="s">
+      <c r="IF17" s="105" t="s">
         <v>682</v>
       </c>
       <c r="IG17" s="48" t="s">
@@ -12773,11 +12785,11 @@
         <v>181</v>
       </c>
     </row>
-    <row r="18" spans="1:248" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:248">
       <c r="A18" s="100"/>
       <c r="B18" s="101"/>
     </row>
-    <row r="19" spans="1:248" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:248">
       <c r="HM19" s="33"/>
       <c r="HN19" s="33"/>
       <c r="HO19" s="33"/>
@@ -12802,961 +12814,961 @@
       <c r="IH19" s="44"/>
       <c r="II19" s="44"/>
     </row>
-    <row r="46" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="47" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="48" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="49" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="50" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="51" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="52" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="53" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="54" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="55" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="56" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="57" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="58" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="59" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="60" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="61" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="62" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="63" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="64" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="65" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="66" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="67" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="68" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="69" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="70" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="71" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="72" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="73" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="74" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="75" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="76" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="77" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="78" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="79" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="80" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="81" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="82" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="83" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="84" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="85" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="86" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="87" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="88" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="89" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="90" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="91" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="92" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="93" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="94" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="95" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="96" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="97" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="98" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="99" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="100" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="101" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="102" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="103" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="104" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="105" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="106" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="107" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="108" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="109" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="110" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="111" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="112" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="113" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="114" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="115" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="116" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="117" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="118" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="119" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="120" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="121" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="122" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="123" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="124" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="125" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="126" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="127" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="128" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="129" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="130" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="131" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="132" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="133" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="134" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="135" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="136" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="137" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="138" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="139" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="140" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="141" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="142" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="143" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="144" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="145" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="146" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="147" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="148" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="149" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="150" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="151" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="152" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="153" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="154" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="155" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="156" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="157" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="158" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="159" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="160" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="161" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="162" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="163" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="164" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="165" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="166" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="167" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="168" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="169" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="170" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="171" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="172" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="173" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="174" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="175" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="176" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="177" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="178" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="179" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="180" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="181" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="182" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="183" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="184" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="185" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="186" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="187" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="188" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="189" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="190" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="191" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="192" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="193" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="194" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="195" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="196" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="197" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="198" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="199" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="200" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="201" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="202" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="203" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="204" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="205" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="206" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="207" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="208" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="209" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="210" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="211" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="212" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="213" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="214" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="215" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="216" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="217" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="218" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="219" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="220" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="221" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="222" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="223" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="224" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="225" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="226" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="227" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="228" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="229" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="230" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="231" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="232" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="233" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="234" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="235" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="236" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="237" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="238" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="239" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="240" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="241" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="242" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="243" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="244" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="245" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="246" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="247" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="248" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="249" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="250" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="251" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="252" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="253" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="254" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="255" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="256" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="257" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="258" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="259" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="260" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="261" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="262" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="263" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="264" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="265" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="266" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="267" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="268" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="269" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="270" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="271" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="272" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="273" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="274" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="275" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="276" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="277" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="278" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="279" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="280" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="281" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="282" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="283" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="284" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="285" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="286" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="287" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="288" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="289" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="290" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="291" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="292" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="293" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="294" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="295" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="296" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="297" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="298" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="299" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="300" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="301" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="302" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="303" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="304" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="305" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="306" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="307" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="308" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="309" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="310" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="311" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="312" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="313" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="314" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="315" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="316" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="317" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="318" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="319" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="320" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="321" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="322" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="323" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="324" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="325" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="326" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="327" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="328" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="329" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="330" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="331" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="332" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="333" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="334" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="335" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="336" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="337" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="338" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="339" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="340" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="341" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="342" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="343" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="344" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="345" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="346" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="347" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="348" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="349" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="350" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="351" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="352" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="353" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="354" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="355" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="356" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="357" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="358" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="359" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="360" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="361" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="362" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="363" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="364" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="365" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="366" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="367" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="368" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="369" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="370" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="371" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="372" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="373" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="374" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="375" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="376" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="377" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="378" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="379" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="380" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="381" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="382" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="383" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="384" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="385" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="386" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="387" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="388" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="389" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="390" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="391" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="392" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="393" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="394" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="395" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="396" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="397" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="398" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="399" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="400" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="401" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="402" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="403" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="404" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="405" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="406" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="407" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="408" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="409" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="410" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="411" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="412" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="413" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="414" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="415" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="416" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="417" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="418" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="419" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="420" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="421" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="422" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="423" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="424" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="425" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="426" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="427" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="428" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="429" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="430" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="431" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="432" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="433" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="434" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="435" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="436" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="437" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="438" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="439" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="440" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="441" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="442" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="443" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="444" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="445" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="446" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="447" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="448" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="449" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="450" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="451" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="452" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="453" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="454" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="455" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="456" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="457" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="458" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="459" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="460" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="461" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="462" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="463" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="464" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="465" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="466" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="467" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="468" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="469" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="470" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="471" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="472" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="473" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="474" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="475" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="476" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="477" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="478" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="479" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="480" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="481" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="482" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="483" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="484" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="485" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="486" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="487" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="488" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="489" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="490" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="491" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="492" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="493" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="494" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="495" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="496" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="497" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="498" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="499" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="500" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="501" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="502" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="503" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="504" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="505" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="506" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="507" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="508" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="509" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="510" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="511" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="512" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="513" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="514" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="515" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="516" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="517" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="518" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="519" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="520" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="521" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="522" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="523" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="524" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="525" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="526" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="527" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="528" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="529" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="530" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="531" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="532" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="533" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="534" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="535" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="536" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="537" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="538" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="539" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="540" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="541" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="542" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="543" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="544" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="545" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="546" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="547" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="548" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="549" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="550" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="551" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="552" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="553" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="554" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="555" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="556" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="557" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="558" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="559" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="560" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="561" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="562" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="563" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="564" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="565" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="566" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="567" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="568" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="569" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="570" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="571" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="572" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="573" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="574" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="575" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="576" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="577" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="578" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="579" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="580" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="581" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="582" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="583" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="584" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="585" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="586" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="587" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="588" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="589" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="590" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="591" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="592" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="593" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="594" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="595" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="596" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="597" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="598" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="599" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="600" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="601" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="602" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="603" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="604" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="605" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="606" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="607" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="608" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="609" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="610" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="611" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="612" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="613" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="614" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="615" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="616" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="617" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="618" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="619" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="620" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="621" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="622" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="623" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="624" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="625" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="626" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="627" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="628" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="629" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="630" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="631" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="632" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="633" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="634" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="635" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="636" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="637" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="638" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="639" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="640" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="641" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="642" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="643" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="644" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="645" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="646" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="647" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="648" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="649" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="650" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="651" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="652" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="653" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="654" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="655" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="656" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="657" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="658" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="659" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="660" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="661" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="662" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="663" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="664" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="665" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="666" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="667" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="668" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="669" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="670" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="671" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="672" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="673" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="674" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="675" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="676" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="677" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="678" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="679" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="680" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="681" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="682" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="683" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="684" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="685" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="686" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="687" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="688" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="689" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="690" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="691" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="692" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="693" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="694" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="695" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="696" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="697" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="698" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="699" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="700" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="701" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="702" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="703" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="704" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="705" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="706" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="707" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="708" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="709" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="710" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="711" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="712" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="713" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="714" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="715" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="716" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="717" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="718" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="719" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="720" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="721" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="722" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="723" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="724" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="725" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="726" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="727" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="728" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="729" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="730" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="731" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="732" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="733" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="734" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="735" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="736" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="737" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="738" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="739" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="740" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="741" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="742" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="743" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="744" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="745" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="746" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="747" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="748" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="749" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="750" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="751" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="752" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="753" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="754" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="755" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="756" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="757" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="758" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="759" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="760" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="761" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="762" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="763" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="764" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="765" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="766" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="767" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="768" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="769" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="770" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="771" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="772" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="773" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="774" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="775" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="776" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="777" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="778" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="779" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="780" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="781" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="782" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="783" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="784" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="785" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="786" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="787" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="788" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="789" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="790" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="791" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="792" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="793" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="794" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="795" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="796" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="797" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="798" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="799" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="800" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="801" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="802" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="803" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="804" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="805" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="806" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="807" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="808" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="809" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="810" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="811" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="812" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="813" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="814" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="815" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="816" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="817" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="818" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="819" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="820" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="821" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="822" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="823" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="824" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="825" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="826" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="827" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="828" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="829" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="830" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="831" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="832" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="833" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="834" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="835" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="836" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="837" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="838" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="839" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="840" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="841" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="842" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="843" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="844" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="845" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="846" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="847" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="848" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="849" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="850" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="851" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="852" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="853" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="854" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="855" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="856" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="857" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="858" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="859" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="860" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="861" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="862" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="863" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="864" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="865" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="866" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="867" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="868" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="869" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="870" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="871" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="872" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="873" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="874" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="875" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="876" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="877" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="878" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="879" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="880" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="881" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="882" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="883" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="884" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="885" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="886" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="887" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="888" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="889" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="890" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="891" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="892" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="893" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="894" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="895" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="896" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="897" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="898" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="899" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="900" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="901" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="902" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="903" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="904" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="905" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="906" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="907" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="908" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="909" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="910" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="911" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="912" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="913" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="914" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="915" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="916" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="917" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="918" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="919" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="920" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="921" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="922" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="923" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="924" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="925" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="926" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="927" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="928" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="929" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="930" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="931" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="932" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="933" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="934" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="935" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="936" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="937" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="938" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="939" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="940" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="941" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="942" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="943" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="944" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="945" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="946" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="947" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="948" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="949" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="950" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="951" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="952" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="953" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="954" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="955" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="956" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="957" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="958" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="959" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="960" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="961" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="962" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="963" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="964" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="965" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="966" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="967" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="968" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="969" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="970" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="971" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="972" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="973" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="974" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="975" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="976" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="977" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="978" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="979" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="980" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="981" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="982" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="983" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="984" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="985" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="986" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="987" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="988" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="989" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="990" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="991" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="992" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="993" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="994" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="995" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="996" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="997" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="998" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="999" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="1000" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="46" ht="12.75"/>
+    <row r="47" ht="12.75"/>
+    <row r="48" ht="12.75"/>
+    <row r="49" ht="12.75"/>
+    <row r="50" ht="12.75"/>
+    <row r="51" ht="12.75"/>
+    <row r="52" ht="12.75"/>
+    <row r="53" ht="12.75"/>
+    <row r="54" ht="12.75"/>
+    <row r="55" ht="12.75"/>
+    <row r="56" ht="12.75"/>
+    <row r="57" ht="12.75"/>
+    <row r="58" ht="12.75"/>
+    <row r="59" ht="12.75"/>
+    <row r="60" ht="12.75"/>
+    <row r="61" ht="12.75"/>
+    <row r="62" ht="12.75"/>
+    <row r="63" ht="12.75"/>
+    <row r="64" ht="12.75"/>
+    <row r="65" ht="12.75"/>
+    <row r="66" ht="12.75"/>
+    <row r="67" ht="12.75"/>
+    <row r="68" ht="12.75"/>
+    <row r="69" ht="12.75"/>
+    <row r="70" ht="12.75"/>
+    <row r="71" ht="12.75"/>
+    <row r="72" ht="12.75"/>
+    <row r="73" ht="12.75"/>
+    <row r="74" ht="12.75"/>
+    <row r="75" ht="12.75"/>
+    <row r="76" ht="12.75"/>
+    <row r="77" ht="12.75"/>
+    <row r="78" ht="12.75"/>
+    <row r="79" ht="12.75"/>
+    <row r="80" ht="12.75"/>
+    <row r="81" ht="12.75"/>
+    <row r="82" ht="12.75"/>
+    <row r="83" ht="12.75"/>
+    <row r="84" ht="12.75"/>
+    <row r="85" ht="12.75"/>
+    <row r="86" ht="12.75"/>
+    <row r="87" ht="12.75"/>
+    <row r="88" ht="12.75"/>
+    <row r="89" ht="12.75"/>
+    <row r="90" ht="12.75"/>
+    <row r="91" ht="12.75"/>
+    <row r="92" ht="12.75"/>
+    <row r="93" ht="12.75"/>
+    <row r="94" ht="12.75"/>
+    <row r="95" ht="12.75"/>
+    <row r="96" ht="12.75"/>
+    <row r="97" ht="12.75"/>
+    <row r="98" ht="12.75"/>
+    <row r="99" ht="12.75"/>
+    <row r="100" ht="12.75"/>
+    <row r="101" ht="12.75"/>
+    <row r="102" ht="12.75"/>
+    <row r="103" ht="12.75"/>
+    <row r="104" ht="12.75"/>
+    <row r="105" ht="12.75"/>
+    <row r="106" ht="12.75"/>
+    <row r="107" ht="12.75"/>
+    <row r="108" ht="12.75"/>
+    <row r="109" ht="12.75"/>
+    <row r="110" ht="12.75"/>
+    <row r="111" ht="12.75"/>
+    <row r="112" ht="12.75"/>
+    <row r="113" ht="12.75"/>
+    <row r="114" ht="12.75"/>
+    <row r="115" ht="12.75"/>
+    <row r="116" ht="12.75"/>
+    <row r="117" ht="12.75"/>
+    <row r="118" ht="12.75"/>
+    <row r="119" ht="12.75"/>
+    <row r="120" ht="12.75"/>
+    <row r="121" ht="12.75"/>
+    <row r="122" ht="12.75"/>
+    <row r="123" ht="12.75"/>
+    <row r="124" ht="12.75"/>
+    <row r="125" ht="12.75"/>
+    <row r="126" ht="12.75"/>
+    <row r="127" ht="12.75"/>
+    <row r="128" ht="12.75"/>
+    <row r="129" ht="12.75"/>
+    <row r="130" ht="12.75"/>
+    <row r="131" ht="12.75"/>
+    <row r="132" ht="12.75"/>
+    <row r="133" ht="12.75"/>
+    <row r="134" ht="12.75"/>
+    <row r="135" ht="12.75"/>
+    <row r="136" ht="12.75"/>
+    <row r="137" ht="12.75"/>
+    <row r="138" ht="12.75"/>
+    <row r="139" ht="12.75"/>
+    <row r="140" ht="12.75"/>
+    <row r="141" ht="12.75"/>
+    <row r="142" ht="12.75"/>
+    <row r="143" ht="12.75"/>
+    <row r="144" ht="12.75"/>
+    <row r="145" ht="12.75"/>
+    <row r="146" ht="12.75"/>
+    <row r="147" ht="12.75"/>
+    <row r="148" ht="12.75"/>
+    <row r="149" ht="12.75"/>
+    <row r="150" ht="12.75"/>
+    <row r="151" ht="12.75"/>
+    <row r="152" ht="12.75"/>
+    <row r="153" ht="12.75"/>
+    <row r="154" ht="12.75"/>
+    <row r="155" ht="12.75"/>
+    <row r="156" ht="12.75"/>
+    <row r="157" ht="12.75"/>
+    <row r="158" ht="12.75"/>
+    <row r="159" ht="12.75"/>
+    <row r="160" ht="12.75"/>
+    <row r="161" ht="12.75"/>
+    <row r="162" ht="12.75"/>
+    <row r="163" ht="12.75"/>
+    <row r="164" ht="12.75"/>
+    <row r="165" ht="12.75"/>
+    <row r="166" ht="12.75"/>
+    <row r="167" ht="12.75"/>
+    <row r="168" ht="12.75"/>
+    <row r="169" ht="12.75"/>
+    <row r="170" ht="12.75"/>
+    <row r="171" ht="12.75"/>
+    <row r="172" ht="12.75"/>
+    <row r="173" ht="12.75"/>
+    <row r="174" ht="12.75"/>
+    <row r="175" ht="12.75"/>
+    <row r="176" ht="12.75"/>
+    <row r="177" ht="12.75"/>
+    <row r="178" ht="12.75"/>
+    <row r="179" ht="12.75"/>
+    <row r="180" ht="12.75"/>
+    <row r="181" ht="12.75"/>
+    <row r="182" ht="12.75"/>
+    <row r="183" ht="12.75"/>
+    <row r="184" ht="12.75"/>
+    <row r="185" ht="12.75"/>
+    <row r="186" ht="12.75"/>
+    <row r="187" ht="12.75"/>
+    <row r="188" ht="12.75"/>
+    <row r="189" ht="12.75"/>
+    <row r="190" ht="12.75"/>
+    <row r="191" ht="12.75"/>
+    <row r="192" ht="12.75"/>
+    <row r="193" ht="12.75"/>
+    <row r="194" ht="12.75"/>
+    <row r="195" ht="12.75"/>
+    <row r="196" ht="12.75"/>
+    <row r="197" ht="12.75"/>
+    <row r="198" ht="12.75"/>
+    <row r="199" ht="12.75"/>
+    <row r="200" ht="12.75"/>
+    <row r="201" ht="12.75"/>
+    <row r="202" ht="12.75"/>
+    <row r="203" ht="12.75"/>
+    <row r="204" ht="12.75"/>
+    <row r="205" ht="12.75"/>
+    <row r="206" ht="12.75"/>
+    <row r="207" ht="12.75"/>
+    <row r="208" ht="12.75"/>
+    <row r="209" ht="12.75"/>
+    <row r="210" ht="12.75"/>
+    <row r="211" ht="12.75"/>
+    <row r="212" ht="12.75"/>
+    <row r="213" ht="12.75"/>
+    <row r="214" ht="12.75"/>
+    <row r="215" ht="12.75"/>
+    <row r="216" ht="12.75"/>
+    <row r="217" ht="12.75"/>
+    <row r="218" ht="12.75"/>
+    <row r="219" ht="12.75"/>
+    <row r="220" ht="12.75"/>
+    <row r="221" ht="12.75"/>
+    <row r="222" ht="12.75"/>
+    <row r="223" ht="12.75"/>
+    <row r="224" ht="12.75"/>
+    <row r="225" ht="12.75"/>
+    <row r="226" ht="12.75"/>
+    <row r="227" ht="12.75"/>
+    <row r="228" ht="12.75"/>
+    <row r="229" ht="12.75"/>
+    <row r="230" ht="12.75"/>
+    <row r="231" ht="12.75"/>
+    <row r="232" ht="12.75"/>
+    <row r="233" ht="12.75"/>
+    <row r="234" ht="12.75"/>
+    <row r="235" ht="12.75"/>
+    <row r="236" ht="12.75"/>
+    <row r="237" ht="12.75"/>
+    <row r="238" ht="12.75"/>
+    <row r="239" ht="12.75"/>
+    <row r="240" ht="12.75"/>
+    <row r="241" ht="12.75"/>
+    <row r="242" ht="12.75"/>
+    <row r="243" ht="12.75"/>
+    <row r="244" ht="12.75"/>
+    <row r="245" ht="12.75"/>
+    <row r="246" ht="12.75"/>
+    <row r="247" ht="12.75"/>
+    <row r="248" ht="12.75"/>
+    <row r="249" ht="12.75"/>
+    <row r="250" ht="12.75"/>
+    <row r="251" ht="12.75"/>
+    <row r="252" ht="12.75"/>
+    <row r="253" ht="12.75"/>
+    <row r="254" ht="12.75"/>
+    <row r="255" ht="12.75"/>
+    <row r="256" ht="12.75"/>
+    <row r="257" ht="12.75"/>
+    <row r="258" ht="12.75"/>
+    <row r="259" ht="12.75"/>
+    <row r="260" ht="12.75"/>
+    <row r="261" ht="12.75"/>
+    <row r="262" ht="12.75"/>
+    <row r="263" ht="12.75"/>
+    <row r="264" ht="12.75"/>
+    <row r="265" ht="12.75"/>
+    <row r="266" ht="12.75"/>
+    <row r="267" ht="12.75"/>
+    <row r="268" ht="12.75"/>
+    <row r="269" ht="12.75"/>
+    <row r="270" ht="12.75"/>
+    <row r="271" ht="12.75"/>
+    <row r="272" ht="12.75"/>
+    <row r="273" ht="12.75"/>
+    <row r="274" ht="12.75"/>
+    <row r="275" ht="12.75"/>
+    <row r="276" ht="12.75"/>
+    <row r="277" ht="12.75"/>
+    <row r="278" ht="12.75"/>
+    <row r="279" ht="12.75"/>
+    <row r="280" ht="12.75"/>
+    <row r="281" ht="12.75"/>
+    <row r="282" ht="12.75"/>
+    <row r="283" ht="12.75"/>
+    <row r="284" ht="12.75"/>
+    <row r="285" ht="12.75"/>
+    <row r="286" ht="12.75"/>
+    <row r="287" ht="12.75"/>
+    <row r="288" ht="12.75"/>
+    <row r="289" ht="12.75"/>
+    <row r="290" ht="12.75"/>
+    <row r="291" ht="12.75"/>
+    <row r="292" ht="12.75"/>
+    <row r="293" ht="12.75"/>
+    <row r="294" ht="12.75"/>
+    <row r="295" ht="12.75"/>
+    <row r="296" ht="12.75"/>
+    <row r="297" ht="12.75"/>
+    <row r="298" ht="12.75"/>
+    <row r="299" ht="12.75"/>
+    <row r="300" ht="12.75"/>
+    <row r="301" ht="12.75"/>
+    <row r="302" ht="12.75"/>
+    <row r="303" ht="12.75"/>
+    <row r="304" ht="12.75"/>
+    <row r="305" ht="12.75"/>
+    <row r="306" ht="12.75"/>
+    <row r="307" ht="12.75"/>
+    <row r="308" ht="12.75"/>
+    <row r="309" ht="12.75"/>
+    <row r="310" ht="12.75"/>
+    <row r="311" ht="12.75"/>
+    <row r="312" ht="12.75"/>
+    <row r="313" ht="12.75"/>
+    <row r="314" ht="12.75"/>
+    <row r="315" ht="12.75"/>
+    <row r="316" ht="12.75"/>
+    <row r="317" ht="12.75"/>
+    <row r="318" ht="12.75"/>
+    <row r="319" ht="12.75"/>
+    <row r="320" ht="12.75"/>
+    <row r="321" ht="12.75"/>
+    <row r="322" ht="12.75"/>
+    <row r="323" ht="12.75"/>
+    <row r="324" ht="12.75"/>
+    <row r="325" ht="12.75"/>
+    <row r="326" ht="12.75"/>
+    <row r="327" ht="12.75"/>
+    <row r="328" ht="12.75"/>
+    <row r="329" ht="12.75"/>
+    <row r="330" ht="12.75"/>
+    <row r="331" ht="12.75"/>
+    <row r="332" ht="12.75"/>
+    <row r="333" ht="12.75"/>
+    <row r="334" ht="12.75"/>
+    <row r="335" ht="12.75"/>
+    <row r="336" ht="12.75"/>
+    <row r="337" ht="12.75"/>
+    <row r="338" ht="12.75"/>
+    <row r="339" ht="12.75"/>
+    <row r="340" ht="12.75"/>
+    <row r="341" ht="12.75"/>
+    <row r="342" ht="12.75"/>
+    <row r="343" ht="12.75"/>
+    <row r="344" ht="12.75"/>
+    <row r="345" ht="12.75"/>
+    <row r="346" ht="12.75"/>
+    <row r="347" ht="12.75"/>
+    <row r="348" ht="12.75"/>
+    <row r="349" ht="12.75"/>
+    <row r="350" ht="12.75"/>
+    <row r="351" ht="12.75"/>
+    <row r="352" ht="12.75"/>
+    <row r="353" ht="12.75"/>
+    <row r="354" ht="12.75"/>
+    <row r="355" ht="12.75"/>
+    <row r="356" ht="12.75"/>
+    <row r="357" ht="12.75"/>
+    <row r="358" ht="12.75"/>
+    <row r="359" ht="12.75"/>
+    <row r="360" ht="12.75"/>
+    <row r="361" ht="12.75"/>
+    <row r="362" ht="12.75"/>
+    <row r="363" ht="12.75"/>
+    <row r="364" ht="12.75"/>
+    <row r="365" ht="12.75"/>
+    <row r="366" ht="12.75"/>
+    <row r="367" ht="12.75"/>
+    <row r="368" ht="12.75"/>
+    <row r="369" ht="12.75"/>
+    <row r="370" ht="12.75"/>
+    <row r="371" ht="12.75"/>
+    <row r="372" ht="12.75"/>
+    <row r="373" ht="12.75"/>
+    <row r="374" ht="12.75"/>
+    <row r="375" ht="12.75"/>
+    <row r="376" ht="12.75"/>
+    <row r="377" ht="12.75"/>
+    <row r="378" ht="12.75"/>
+    <row r="379" ht="12.75"/>
+    <row r="380" ht="12.75"/>
+    <row r="381" ht="12.75"/>
+    <row r="382" ht="12.75"/>
+    <row r="383" ht="12.75"/>
+    <row r="384" ht="12.75"/>
+    <row r="385" ht="12.75"/>
+    <row r="386" ht="12.75"/>
+    <row r="387" ht="12.75"/>
+    <row r="388" ht="12.75"/>
+    <row r="389" ht="12.75"/>
+    <row r="390" ht="12.75"/>
+    <row r="391" ht="12.75"/>
+    <row r="392" ht="12.75"/>
+    <row r="393" ht="12.75"/>
+    <row r="394" ht="12.75"/>
+    <row r="395" ht="12.75"/>
+    <row r="396" ht="12.75"/>
+    <row r="397" ht="12.75"/>
+    <row r="398" ht="12.75"/>
+    <row r="399" ht="12.75"/>
+    <row r="400" ht="12.75"/>
+    <row r="401" ht="12.75"/>
+    <row r="402" ht="12.75"/>
+    <row r="403" ht="12.75"/>
+    <row r="404" ht="12.75"/>
+    <row r="405" ht="12.75"/>
+    <row r="406" ht="12.75"/>
+    <row r="407" ht="12.75"/>
+    <row r="408" ht="12.75"/>
+    <row r="409" ht="12.75"/>
+    <row r="410" ht="12.75"/>
+    <row r="411" ht="12.75"/>
+    <row r="412" ht="12.75"/>
+    <row r="413" ht="12.75"/>
+    <row r="414" ht="12.75"/>
+    <row r="415" ht="12.75"/>
+    <row r="416" ht="12.75"/>
+    <row r="417" ht="12.75"/>
+    <row r="418" ht="12.75"/>
+    <row r="419" ht="12.75"/>
+    <row r="420" ht="12.75"/>
+    <row r="421" ht="12.75"/>
+    <row r="422" ht="12.75"/>
+    <row r="423" ht="12.75"/>
+    <row r="424" ht="12.75"/>
+    <row r="425" ht="12.75"/>
+    <row r="426" ht="12.75"/>
+    <row r="427" ht="12.75"/>
+    <row r="428" ht="12.75"/>
+    <row r="429" ht="12.75"/>
+    <row r="430" ht="12.75"/>
+    <row r="431" ht="12.75"/>
+    <row r="432" ht="12.75"/>
+    <row r="433" ht="12.75"/>
+    <row r="434" ht="12.75"/>
+    <row r="435" ht="12.75"/>
+    <row r="436" ht="12.75"/>
+    <row r="437" ht="12.75"/>
+    <row r="438" ht="12.75"/>
+    <row r="439" ht="12.75"/>
+    <row r="440" ht="12.75"/>
+    <row r="441" ht="12.75"/>
+    <row r="442" ht="12.75"/>
+    <row r="443" ht="12.75"/>
+    <row r="444" ht="12.75"/>
+    <row r="445" ht="12.75"/>
+    <row r="446" ht="12.75"/>
+    <row r="447" ht="12.75"/>
+    <row r="448" ht="12.75"/>
+    <row r="449" ht="12.75"/>
+    <row r="450" ht="12.75"/>
+    <row r="451" ht="12.75"/>
+    <row r="452" ht="12.75"/>
+    <row r="453" ht="12.75"/>
+    <row r="454" ht="12.75"/>
+    <row r="455" ht="12.75"/>
+    <row r="456" ht="12.75"/>
+    <row r="457" ht="12.75"/>
+    <row r="458" ht="12.75"/>
+    <row r="459" ht="12.75"/>
+    <row r="460" ht="12.75"/>
+    <row r="461" ht="12.75"/>
+    <row r="462" ht="12.75"/>
+    <row r="463" ht="12.75"/>
+    <row r="464" ht="12.75"/>
+    <row r="465" ht="12.75"/>
+    <row r="466" ht="12.75"/>
+    <row r="467" ht="12.75"/>
+    <row r="468" ht="12.75"/>
+    <row r="469" ht="12.75"/>
+    <row r="470" ht="12.75"/>
+    <row r="471" ht="12.75"/>
+    <row r="472" ht="12.75"/>
+    <row r="473" ht="12.75"/>
+    <row r="474" ht="12.75"/>
+    <row r="475" ht="12.75"/>
+    <row r="476" ht="12.75"/>
+    <row r="477" ht="12.75"/>
+    <row r="478" ht="12.75"/>
+    <row r="479" ht="12.75"/>
+    <row r="480" ht="12.75"/>
+    <row r="481" ht="12.75"/>
+    <row r="482" ht="12.75"/>
+    <row r="483" ht="12.75"/>
+    <row r="484" ht="12.75"/>
+    <row r="485" ht="12.75"/>
+    <row r="486" ht="12.75"/>
+    <row r="487" ht="12.75"/>
+    <row r="488" ht="12.75"/>
+    <row r="489" ht="12.75"/>
+    <row r="490" ht="12.75"/>
+    <row r="491" ht="12.75"/>
+    <row r="492" ht="12.75"/>
+    <row r="493" ht="12.75"/>
+    <row r="494" ht="12.75"/>
+    <row r="495" ht="12.75"/>
+    <row r="496" ht="12.75"/>
+    <row r="497" ht="12.75"/>
+    <row r="498" ht="12.75"/>
+    <row r="499" ht="12.75"/>
+    <row r="500" ht="12.75"/>
+    <row r="501" ht="12.75"/>
+    <row r="502" ht="12.75"/>
+    <row r="503" ht="12.75"/>
+    <row r="504" ht="12.75"/>
+    <row r="505" ht="12.75"/>
+    <row r="506" ht="12.75"/>
+    <row r="507" ht="12.75"/>
+    <row r="508" ht="12.75"/>
+    <row r="509" ht="12.75"/>
+    <row r="510" ht="12.75"/>
+    <row r="511" ht="12.75"/>
+    <row r="512" ht="12.75"/>
+    <row r="513" ht="12.75"/>
+    <row r="514" ht="12.75"/>
+    <row r="515" ht="12.75"/>
+    <row r="516" ht="12.75"/>
+    <row r="517" ht="12.75"/>
+    <row r="518" ht="12.75"/>
+    <row r="519" ht="12.75"/>
+    <row r="520" ht="12.75"/>
+    <row r="521" ht="12.75"/>
+    <row r="522" ht="12.75"/>
+    <row r="523" ht="12.75"/>
+    <row r="524" ht="12.75"/>
+    <row r="525" ht="12.75"/>
+    <row r="526" ht="12.75"/>
+    <row r="527" ht="12.75"/>
+    <row r="528" ht="12.75"/>
+    <row r="529" ht="12.75"/>
+    <row r="530" ht="12.75"/>
+    <row r="531" ht="12.75"/>
+    <row r="532" ht="12.75"/>
+    <row r="533" ht="12.75"/>
+    <row r="534" ht="12.75"/>
+    <row r="535" ht="12.75"/>
+    <row r="536" ht="12.75"/>
+    <row r="537" ht="12.75"/>
+    <row r="538" ht="12.75"/>
+    <row r="539" ht="12.75"/>
+    <row r="540" ht="12.75"/>
+    <row r="541" ht="12.75"/>
+    <row r="542" ht="12.75"/>
+    <row r="543" ht="12.75"/>
+    <row r="544" ht="12.75"/>
+    <row r="545" ht="12.75"/>
+    <row r="546" ht="12.75"/>
+    <row r="547" ht="12.75"/>
+    <row r="548" ht="12.75"/>
+    <row r="549" ht="12.75"/>
+    <row r="550" ht="12.75"/>
+    <row r="551" ht="12.75"/>
+    <row r="552" ht="12.75"/>
+    <row r="553" ht="12.75"/>
+    <row r="554" ht="12.75"/>
+    <row r="555" ht="12.75"/>
+    <row r="556" ht="12.75"/>
+    <row r="557" ht="12.75"/>
+    <row r="558" ht="12.75"/>
+    <row r="559" ht="12.75"/>
+    <row r="560" ht="12.75"/>
+    <row r="561" ht="12.75"/>
+    <row r="562" ht="12.75"/>
+    <row r="563" ht="12.75"/>
+    <row r="564" ht="12.75"/>
+    <row r="565" ht="12.75"/>
+    <row r="566" ht="12.75"/>
+    <row r="567" ht="12.75"/>
+    <row r="568" ht="12.75"/>
+    <row r="569" ht="12.75"/>
+    <row r="570" ht="12.75"/>
+    <row r="571" ht="12.75"/>
+    <row r="572" ht="12.75"/>
+    <row r="573" ht="12.75"/>
+    <row r="574" ht="12.75"/>
+    <row r="575" ht="12.75"/>
+    <row r="576" ht="12.75"/>
+    <row r="577" ht="12.75"/>
+    <row r="578" ht="12.75"/>
+    <row r="579" ht="12.75"/>
+    <row r="580" ht="12.75"/>
+    <row r="581" ht="12.75"/>
+    <row r="582" ht="12.75"/>
+    <row r="583" ht="12.75"/>
+    <row r="584" ht="12.75"/>
+    <row r="585" ht="12.75"/>
+    <row r="586" ht="12.75"/>
+    <row r="587" ht="12.75"/>
+    <row r="588" ht="12.75"/>
+    <row r="589" ht="12.75"/>
+    <row r="590" ht="12.75"/>
+    <row r="591" ht="12.75"/>
+    <row r="592" ht="12.75"/>
+    <row r="593" ht="12.75"/>
+    <row r="594" ht="12.75"/>
+    <row r="595" ht="12.75"/>
+    <row r="596" ht="12.75"/>
+    <row r="597" ht="12.75"/>
+    <row r="598" ht="12.75"/>
+    <row r="599" ht="12.75"/>
+    <row r="600" ht="12.75"/>
+    <row r="601" ht="12.75"/>
+    <row r="602" ht="12.75"/>
+    <row r="603" ht="12.75"/>
+    <row r="604" ht="12.75"/>
+    <row r="605" ht="12.75"/>
+    <row r="606" ht="12.75"/>
+    <row r="607" ht="12.75"/>
+    <row r="608" ht="12.75"/>
+    <row r="609" ht="12.75"/>
+    <row r="610" ht="12.75"/>
+    <row r="611" ht="12.75"/>
+    <row r="612" ht="12.75"/>
+    <row r="613" ht="12.75"/>
+    <row r="614" ht="12.75"/>
+    <row r="615" ht="12.75"/>
+    <row r="616" ht="12.75"/>
+    <row r="617" ht="12.75"/>
+    <row r="618" ht="12.75"/>
+    <row r="619" ht="12.75"/>
+    <row r="620" ht="12.75"/>
+    <row r="621" ht="12.75"/>
+    <row r="622" ht="12.75"/>
+    <row r="623" ht="12.75"/>
+    <row r="624" ht="12.75"/>
+    <row r="625" ht="12.75"/>
+    <row r="626" ht="12.75"/>
+    <row r="627" ht="12.75"/>
+    <row r="628" ht="12.75"/>
+    <row r="629" ht="12.75"/>
+    <row r="630" ht="12.75"/>
+    <row r="631" ht="12.75"/>
+    <row r="632" ht="12.75"/>
+    <row r="633" ht="12.75"/>
+    <row r="634" ht="12.75"/>
+    <row r="635" ht="12.75"/>
+    <row r="636" ht="12.75"/>
+    <row r="637" ht="12.75"/>
+    <row r="638" ht="12.75"/>
+    <row r="639" ht="12.75"/>
+    <row r="640" ht="12.75"/>
+    <row r="641" ht="12.75"/>
+    <row r="642" ht="12.75"/>
+    <row r="643" ht="12.75"/>
+    <row r="644" ht="12.75"/>
+    <row r="645" ht="12.75"/>
+    <row r="646" ht="12.75"/>
+    <row r="647" ht="12.75"/>
+    <row r="648" ht="12.75"/>
+    <row r="649" ht="12.75"/>
+    <row r="650" ht="12.75"/>
+    <row r="651" ht="12.75"/>
+    <row r="652" ht="12.75"/>
+    <row r="653" ht="12.75"/>
+    <row r="654" ht="12.75"/>
+    <row r="655" ht="12.75"/>
+    <row r="656" ht="12.75"/>
+    <row r="657" ht="12.75"/>
+    <row r="658" ht="12.75"/>
+    <row r="659" ht="12.75"/>
+    <row r="660" ht="12.75"/>
+    <row r="661" ht="12.75"/>
+    <row r="662" ht="12.75"/>
+    <row r="663" ht="12.75"/>
+    <row r="664" ht="12.75"/>
+    <row r="665" ht="12.75"/>
+    <row r="666" ht="12.75"/>
+    <row r="667" ht="12.75"/>
+    <row r="668" ht="12.75"/>
+    <row r="669" ht="12.75"/>
+    <row r="670" ht="12.75"/>
+    <row r="671" ht="12.75"/>
+    <row r="672" ht="12.75"/>
+    <row r="673" ht="12.75"/>
+    <row r="674" ht="12.75"/>
+    <row r="675" ht="12.75"/>
+    <row r="676" ht="12.75"/>
+    <row r="677" ht="12.75"/>
+    <row r="678" ht="12.75"/>
+    <row r="679" ht="12.75"/>
+    <row r="680" ht="12.75"/>
+    <row r="681" ht="12.75"/>
+    <row r="682" ht="12.75"/>
+    <row r="683" ht="12.75"/>
+    <row r="684" ht="12.75"/>
+    <row r="685" ht="12.75"/>
+    <row r="686" ht="12.75"/>
+    <row r="687" ht="12.75"/>
+    <row r="688" ht="12.75"/>
+    <row r="689" ht="12.75"/>
+    <row r="690" ht="12.75"/>
+    <row r="691" ht="12.75"/>
+    <row r="692" ht="12.75"/>
+    <row r="693" ht="12.75"/>
+    <row r="694" ht="12.75"/>
+    <row r="695" ht="12.75"/>
+    <row r="696" ht="12.75"/>
+    <row r="697" ht="12.75"/>
+    <row r="698" ht="12.75"/>
+    <row r="699" ht="12.75"/>
+    <row r="700" ht="12.75"/>
+    <row r="701" ht="12.75"/>
+    <row r="702" ht="12.75"/>
+    <row r="703" ht="12.75"/>
+    <row r="704" ht="12.75"/>
+    <row r="705" ht="12.75"/>
+    <row r="706" ht="12.75"/>
+    <row r="707" ht="12.75"/>
+    <row r="708" ht="12.75"/>
+    <row r="709" ht="12.75"/>
+    <row r="710" ht="12.75"/>
+    <row r="711" ht="12.75"/>
+    <row r="712" ht="12.75"/>
+    <row r="713" ht="12.75"/>
+    <row r="714" ht="12.75"/>
+    <row r="715" ht="12.75"/>
+    <row r="716" ht="12.75"/>
+    <row r="717" ht="12.75"/>
+    <row r="718" ht="12.75"/>
+    <row r="719" ht="12.75"/>
+    <row r="720" ht="12.75"/>
+    <row r="721" ht="12.75"/>
+    <row r="722" ht="12.75"/>
+    <row r="723" ht="12.75"/>
+    <row r="724" ht="12.75"/>
+    <row r="725" ht="12.75"/>
+    <row r="726" ht="12.75"/>
+    <row r="727" ht="12.75"/>
+    <row r="728" ht="12.75"/>
+    <row r="729" ht="12.75"/>
+    <row r="730" ht="12.75"/>
+    <row r="731" ht="12.75"/>
+    <row r="732" ht="12.75"/>
+    <row r="733" ht="12.75"/>
+    <row r="734" ht="12.75"/>
+    <row r="735" ht="12.75"/>
+    <row r="736" ht="12.75"/>
+    <row r="737" ht="12.75"/>
+    <row r="738" ht="12.75"/>
+    <row r="739" ht="12.75"/>
+    <row r="740" ht="12.75"/>
+    <row r="741" ht="12.75"/>
+    <row r="742" ht="12.75"/>
+    <row r="743" ht="12.75"/>
+    <row r="744" ht="12.75"/>
+    <row r="745" ht="12.75"/>
+    <row r="746" ht="12.75"/>
+    <row r="747" ht="12.75"/>
+    <row r="748" ht="12.75"/>
+    <row r="749" ht="12.75"/>
+    <row r="750" ht="12.75"/>
+    <row r="751" ht="12.75"/>
+    <row r="752" ht="12.75"/>
+    <row r="753" ht="12.75"/>
+    <row r="754" ht="12.75"/>
+    <row r="755" ht="12.75"/>
+    <row r="756" ht="12.75"/>
+    <row r="757" ht="12.75"/>
+    <row r="758" ht="12.75"/>
+    <row r="759" ht="12.75"/>
+    <row r="760" ht="12.75"/>
+    <row r="761" ht="12.75"/>
+    <row r="762" ht="12.75"/>
+    <row r="763" ht="12.75"/>
+    <row r="764" ht="12.75"/>
+    <row r="765" ht="12.75"/>
+    <row r="766" ht="12.75"/>
+    <row r="767" ht="12.75"/>
+    <row r="768" ht="12.75"/>
+    <row r="769" ht="12.75"/>
+    <row r="770" ht="12.75"/>
+    <row r="771" ht="12.75"/>
+    <row r="772" ht="12.75"/>
+    <row r="773" ht="12.75"/>
+    <row r="774" ht="12.75"/>
+    <row r="775" ht="12.75"/>
+    <row r="776" ht="12.75"/>
+    <row r="777" ht="12.75"/>
+    <row r="778" ht="12.75"/>
+    <row r="779" ht="12.75"/>
+    <row r="780" ht="12.75"/>
+    <row r="781" ht="12.75"/>
+    <row r="782" ht="12.75"/>
+    <row r="783" ht="12.75"/>
+    <row r="784" ht="12.75"/>
+    <row r="785" ht="12.75"/>
+    <row r="786" ht="12.75"/>
+    <row r="787" ht="12.75"/>
+    <row r="788" ht="12.75"/>
+    <row r="789" ht="12.75"/>
+    <row r="790" ht="12.75"/>
+    <row r="791" ht="12.75"/>
+    <row r="792" ht="12.75"/>
+    <row r="793" ht="12.75"/>
+    <row r="794" ht="12.75"/>
+    <row r="795" ht="12.75"/>
+    <row r="796" ht="12.75"/>
+    <row r="797" ht="12.75"/>
+    <row r="798" ht="12.75"/>
+    <row r="799" ht="12.75"/>
+    <row r="800" ht="12.75"/>
+    <row r="801" ht="12.75"/>
+    <row r="802" ht="12.75"/>
+    <row r="803" ht="12.75"/>
+    <row r="804" ht="12.75"/>
+    <row r="805" ht="12.75"/>
+    <row r="806" ht="12.75"/>
+    <row r="807" ht="12.75"/>
+    <row r="808" ht="12.75"/>
+    <row r="809" ht="12.75"/>
+    <row r="810" ht="12.75"/>
+    <row r="811" ht="12.75"/>
+    <row r="812" ht="12.75"/>
+    <row r="813" ht="12.75"/>
+    <row r="814" ht="12.75"/>
+    <row r="815" ht="12.75"/>
+    <row r="816" ht="12.75"/>
+    <row r="817" ht="12.75"/>
+    <row r="818" ht="12.75"/>
+    <row r="819" ht="12.75"/>
+    <row r="820" ht="12.75"/>
+    <row r="821" ht="12.75"/>
+    <row r="822" ht="12.75"/>
+    <row r="823" ht="12.75"/>
+    <row r="824" ht="12.75"/>
+    <row r="825" ht="12.75"/>
+    <row r="826" ht="12.75"/>
+    <row r="827" ht="12.75"/>
+    <row r="828" ht="12.75"/>
+    <row r="829" ht="12.75"/>
+    <row r="830" ht="12.75"/>
+    <row r="831" ht="12.75"/>
+    <row r="832" ht="12.75"/>
+    <row r="833" ht="12.75"/>
+    <row r="834" ht="12.75"/>
+    <row r="835" ht="12.75"/>
+    <row r="836" ht="12.75"/>
+    <row r="837" ht="12.75"/>
+    <row r="838" ht="12.75"/>
+    <row r="839" ht="12.75"/>
+    <row r="840" ht="12.75"/>
+    <row r="841" ht="12.75"/>
+    <row r="842" ht="12.75"/>
+    <row r="843" ht="12.75"/>
+    <row r="844" ht="12.75"/>
+    <row r="845" ht="12.75"/>
+    <row r="846" ht="12.75"/>
+    <row r="847" ht="12.75"/>
+    <row r="848" ht="12.75"/>
+    <row r="849" ht="12.75"/>
+    <row r="850" ht="12.75"/>
+    <row r="851" ht="12.75"/>
+    <row r="852" ht="12.75"/>
+    <row r="853" ht="12.75"/>
+    <row r="854" ht="12.75"/>
+    <row r="855" ht="12.75"/>
+    <row r="856" ht="12.75"/>
+    <row r="857" ht="12.75"/>
+    <row r="858" ht="12.75"/>
+    <row r="859" ht="12.75"/>
+    <row r="860" ht="12.75"/>
+    <row r="861" ht="12.75"/>
+    <row r="862" ht="12.75"/>
+    <row r="863" ht="12.75"/>
+    <row r="864" ht="12.75"/>
+    <row r="865" ht="12.75"/>
+    <row r="866" ht="12.75"/>
+    <row r="867" ht="12.75"/>
+    <row r="868" ht="12.75"/>
+    <row r="869" ht="12.75"/>
+    <row r="870" ht="12.75"/>
+    <row r="871" ht="12.75"/>
+    <row r="872" ht="12.75"/>
+    <row r="873" ht="12.75"/>
+    <row r="874" ht="12.75"/>
+    <row r="875" ht="12.75"/>
+    <row r="876" ht="12.75"/>
+    <row r="877" ht="12.75"/>
+    <row r="878" ht="12.75"/>
+    <row r="879" ht="12.75"/>
+    <row r="880" ht="12.75"/>
+    <row r="881" ht="12.75"/>
+    <row r="882" ht="12.75"/>
+    <row r="883" ht="12.75"/>
+    <row r="884" ht="12.75"/>
+    <row r="885" ht="12.75"/>
+    <row r="886" ht="12.75"/>
+    <row r="887" ht="12.75"/>
+    <row r="888" ht="12.75"/>
+    <row r="889" ht="12.75"/>
+    <row r="890" ht="12.75"/>
+    <row r="891" ht="12.75"/>
+    <row r="892" ht="12.75"/>
+    <row r="893" ht="12.75"/>
+    <row r="894" ht="12.75"/>
+    <row r="895" ht="12.75"/>
+    <row r="896" ht="12.75"/>
+    <row r="897" ht="12.75"/>
+    <row r="898" ht="12.75"/>
+    <row r="899" ht="12.75"/>
+    <row r="900" ht="12.75"/>
+    <row r="901" ht="12.75"/>
+    <row r="902" ht="12.75"/>
+    <row r="903" ht="12.75"/>
+    <row r="904" ht="12.75"/>
+    <row r="905" ht="12.75"/>
+    <row r="906" ht="12.75"/>
+    <row r="907" ht="12.75"/>
+    <row r="908" ht="12.75"/>
+    <row r="909" ht="12.75"/>
+    <row r="910" ht="12.75"/>
+    <row r="911" ht="12.75"/>
+    <row r="912" ht="12.75"/>
+    <row r="913" ht="12.75"/>
+    <row r="914" ht="12.75"/>
+    <row r="915" ht="12.75"/>
+    <row r="916" ht="12.75"/>
+    <row r="917" ht="12.75"/>
+    <row r="918" ht="12.75"/>
+    <row r="919" ht="12.75"/>
+    <row r="920" ht="12.75"/>
+    <row r="921" ht="12.75"/>
+    <row r="922" ht="12.75"/>
+    <row r="923" ht="12.75"/>
+    <row r="924" ht="12.75"/>
+    <row r="925" ht="12.75"/>
+    <row r="926" ht="12.75"/>
+    <row r="927" ht="12.75"/>
+    <row r="928" ht="12.75"/>
+    <row r="929" ht="12.75"/>
+    <row r="930" ht="12.75"/>
+    <row r="931" ht="12.75"/>
+    <row r="932" ht="12.75"/>
+    <row r="933" ht="12.75"/>
+    <row r="934" ht="12.75"/>
+    <row r="935" ht="12.75"/>
+    <row r="936" ht="12.75"/>
+    <row r="937" ht="12.75"/>
+    <row r="938" ht="12.75"/>
+    <row r="939" ht="12.75"/>
+    <row r="940" ht="12.75"/>
+    <row r="941" ht="12.75"/>
+    <row r="942" ht="12.75"/>
+    <row r="943" ht="12.75"/>
+    <row r="944" ht="12.75"/>
+    <row r="945" ht="12.75"/>
+    <row r="946" ht="12.75"/>
+    <row r="947" ht="12.75"/>
+    <row r="948" ht="12.75"/>
+    <row r="949" ht="12.75"/>
+    <row r="950" ht="12.75"/>
+    <row r="951" ht="12.75"/>
+    <row r="952" ht="12.75"/>
+    <row r="953" ht="12.75"/>
+    <row r="954" ht="12.75"/>
+    <row r="955" ht="12.75"/>
+    <row r="956" ht="12.75"/>
+    <row r="957" ht="12.75"/>
+    <row r="958" ht="12.75"/>
+    <row r="959" ht="12.75"/>
+    <row r="960" ht="12.75"/>
+    <row r="961" ht="12.75"/>
+    <row r="962" ht="12.75"/>
+    <row r="963" ht="12.75"/>
+    <row r="964" ht="12.75"/>
+    <row r="965" ht="12.75"/>
+    <row r="966" ht="12.75"/>
+    <row r="967" ht="12.75"/>
+    <row r="968" ht="12.75"/>
+    <row r="969" ht="12.75"/>
+    <row r="970" ht="12.75"/>
+    <row r="971" ht="12.75"/>
+    <row r="972" ht="12.75"/>
+    <row r="973" ht="12.75"/>
+    <row r="974" ht="12.75"/>
+    <row r="975" ht="12.75"/>
+    <row r="976" ht="12.75"/>
+    <row r="977" ht="12.75"/>
+    <row r="978" ht="12.75"/>
+    <row r="979" ht="12.75"/>
+    <row r="980" ht="12.75"/>
+    <row r="981" ht="12.75"/>
+    <row r="982" ht="12.75"/>
+    <row r="983" ht="12.75"/>
+    <row r="984" ht="12.75"/>
+    <row r="985" ht="12.75"/>
+    <row r="986" ht="12.75"/>
+    <row r="987" ht="12.75"/>
+    <row r="988" ht="12.75"/>
+    <row r="989" ht="12.75"/>
+    <row r="990" ht="12.75"/>
+    <row r="991" ht="12.75"/>
+    <row r="992" ht="12.75"/>
+    <row r="993" ht="12.75"/>
+    <row r="994" ht="12.75"/>
+    <row r="995" ht="12.75"/>
+    <row r="996" ht="12.75"/>
+    <row r="997" ht="12.75"/>
+    <row r="998" ht="12.75"/>
+    <row r="999" ht="12.75"/>
+    <row r="1000" ht="12.75"/>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="HM1:HN1"/>
@@ -13786,8 +13798,8 @@
     <hyperlink ref="BP3" r:id="rId13"/>
     <hyperlink ref="CC3" r:id="rId14"/>
     <hyperlink ref="CD3" r:id="rId15"/>
-    <hyperlink ref="CH3" r:id="rId16"/>
-    <hyperlink ref="CI3" r:id="rId17"/>
+    <hyperlink ref="CH3" r:id="rId16" display="http://id.loc.gov/vocabulary/languages"/>
+    <hyperlink ref="CI3" r:id="rId17" display="http://id.loc.gov/vocabulary/languages/eng"/>
     <hyperlink ref="CL3" r:id="rId18"/>
     <hyperlink ref="CM3" r:id="rId19"/>
     <hyperlink ref="HP3" r:id="rId20"/>
@@ -13815,480 +13827,480 @@
     <hyperlink ref="BP4" r:id="rId42"/>
     <hyperlink ref="CC4" r:id="rId43"/>
     <hyperlink ref="CD4" r:id="rId44"/>
-    <hyperlink ref="CH4" r:id="rId45"/>
-    <hyperlink ref="CI4" r:id="rId46"/>
-    <hyperlink ref="CL4" r:id="rId47"/>
-    <hyperlink ref="CM4" r:id="rId48"/>
-    <hyperlink ref="DY4" r:id="rId49"/>
-    <hyperlink ref="DZ4" r:id="rId50"/>
-    <hyperlink ref="EE4" r:id="rId51"/>
-    <hyperlink ref="ER4" r:id="rId52"/>
-    <hyperlink ref="FO4" r:id="rId53"/>
-    <hyperlink ref="GF4" r:id="rId54"/>
-    <hyperlink ref="GG4" r:id="rId55"/>
-    <hyperlink ref="HP4" r:id="rId56"/>
-    <hyperlink ref="HS4" r:id="rId57"/>
-    <hyperlink ref="HY4" r:id="rId58"/>
-    <hyperlink ref="HZ4" r:id="rId59"/>
-    <hyperlink ref="IH4" r:id="rId60"/>
-    <hyperlink ref="II4" r:id="rId61"/>
-    <hyperlink ref="IL4" r:id="rId62"/>
-    <hyperlink ref="IM4" r:id="rId63"/>
-    <hyperlink ref="L5" r:id="rId64"/>
-    <hyperlink ref="Q5" r:id="rId65"/>
-    <hyperlink ref="R5" r:id="rId66"/>
-    <hyperlink ref="V5" r:id="rId67"/>
-    <hyperlink ref="W5" r:id="rId68"/>
-    <hyperlink ref="AF5" r:id="rId69"/>
-    <hyperlink ref="AK5" r:id="rId70"/>
-    <hyperlink ref="AL5" r:id="rId71"/>
-    <hyperlink ref="AP5" r:id="rId72"/>
-    <hyperlink ref="AU5" r:id="rId73"/>
-    <hyperlink ref="AV5" r:id="rId74"/>
-    <hyperlink ref="AZ5" r:id="rId75"/>
-    <hyperlink ref="BE5" r:id="rId76"/>
-    <hyperlink ref="BF5" r:id="rId77"/>
-    <hyperlink ref="BP5" r:id="rId78"/>
-    <hyperlink ref="CC5" r:id="rId79"/>
-    <hyperlink ref="CD5" r:id="rId80"/>
-    <hyperlink ref="CH5" r:id="rId81"/>
-    <hyperlink ref="CI5" r:id="rId82"/>
-    <hyperlink ref="CL5" r:id="rId83"/>
-    <hyperlink ref="CM5" r:id="rId84"/>
-    <hyperlink ref="DU5" r:id="rId85"/>
-    <hyperlink ref="EQ5" r:id="rId86"/>
-    <hyperlink ref="ER5" r:id="rId87"/>
-    <hyperlink ref="HP5" r:id="rId88"/>
-    <hyperlink ref="HS5" r:id="rId89"/>
-    <hyperlink ref="HY5" r:id="rId90"/>
-    <hyperlink ref="HZ5" r:id="rId91"/>
-    <hyperlink ref="IH5" r:id="rId92"/>
-    <hyperlink ref="II5" r:id="rId93"/>
-    <hyperlink ref="IL5" r:id="rId94"/>
-    <hyperlink ref="IM5" r:id="rId95"/>
-    <hyperlink ref="L6" r:id="rId96"/>
-    <hyperlink ref="Q6" r:id="rId97"/>
-    <hyperlink ref="R6" r:id="rId98"/>
-    <hyperlink ref="V6" r:id="rId99"/>
-    <hyperlink ref="W6" r:id="rId100"/>
-    <hyperlink ref="AA6" r:id="rId101"/>
-    <hyperlink ref="AB6" r:id="rId102"/>
-    <hyperlink ref="AF6" r:id="rId103"/>
-    <hyperlink ref="AK6" r:id="rId104"/>
-    <hyperlink ref="AL6" r:id="rId105"/>
-    <hyperlink ref="AP6" r:id="rId106"/>
-    <hyperlink ref="AU6" r:id="rId107"/>
-    <hyperlink ref="AV6" r:id="rId108"/>
-    <hyperlink ref="AZ6" r:id="rId109"/>
-    <hyperlink ref="BE6" r:id="rId110"/>
-    <hyperlink ref="BF6" r:id="rId111"/>
-    <hyperlink ref="BP6" r:id="rId112"/>
-    <hyperlink ref="CC6" r:id="rId113"/>
-    <hyperlink ref="CD6" r:id="rId114"/>
-    <hyperlink ref="CH6" r:id="rId115"/>
-    <hyperlink ref="CI6" r:id="rId116"/>
-    <hyperlink ref="CL6" r:id="rId117"/>
-    <hyperlink ref="CM6" r:id="rId118"/>
-    <hyperlink ref="DY6" r:id="rId119"/>
-    <hyperlink ref="DZ6" r:id="rId120"/>
-    <hyperlink ref="EE6" r:id="rId121"/>
-    <hyperlink ref="ER6" r:id="rId122"/>
-    <hyperlink ref="HP6" r:id="rId123"/>
-    <hyperlink ref="HS6" r:id="rId124"/>
-    <hyperlink ref="HY6" r:id="rId125"/>
-    <hyperlink ref="HZ6" r:id="rId126"/>
-    <hyperlink ref="IH6" r:id="rId127"/>
-    <hyperlink ref="II6" r:id="rId128"/>
-    <hyperlink ref="IL6" r:id="rId129"/>
-    <hyperlink ref="IM6" r:id="rId130"/>
-    <hyperlink ref="L7" r:id="rId131"/>
-    <hyperlink ref="Q7" r:id="rId132"/>
-    <hyperlink ref="R7" r:id="rId133"/>
-    <hyperlink ref="V7" r:id="rId134"/>
-    <hyperlink ref="W7" r:id="rId135"/>
-    <hyperlink ref="AF7" r:id="rId136"/>
-    <hyperlink ref="AK7" r:id="rId137"/>
-    <hyperlink ref="AL7" r:id="rId138"/>
-    <hyperlink ref="AP7" r:id="rId139"/>
-    <hyperlink ref="AU7" r:id="rId140"/>
-    <hyperlink ref="AV7" r:id="rId141"/>
-    <hyperlink ref="AZ7" r:id="rId142"/>
-    <hyperlink ref="BP7" r:id="rId143"/>
-    <hyperlink ref="CC7" r:id="rId144"/>
-    <hyperlink ref="CD7" r:id="rId145"/>
-    <hyperlink ref="CH7" r:id="rId146"/>
-    <hyperlink ref="CI7" r:id="rId147"/>
-    <hyperlink ref="CL7" r:id="rId148"/>
-    <hyperlink ref="CM7" r:id="rId149"/>
-    <hyperlink ref="DT7" r:id="rId150"/>
-    <hyperlink ref="DU7" r:id="rId151"/>
-    <hyperlink ref="ER7" r:id="rId152"/>
-    <hyperlink ref="FO7" r:id="rId153"/>
-    <hyperlink ref="FT7" r:id="rId154"/>
-    <hyperlink ref="GG7" r:id="rId155"/>
-    <hyperlink ref="GL7" r:id="rId156"/>
-    <hyperlink ref="GY7" r:id="rId157"/>
-    <hyperlink ref="HD7" r:id="rId158"/>
-    <hyperlink ref="HP7" r:id="rId159"/>
-    <hyperlink ref="HS7" r:id="rId160"/>
-    <hyperlink ref="HY7" r:id="rId161"/>
-    <hyperlink ref="HZ7" r:id="rId162"/>
-    <hyperlink ref="IH7" r:id="rId163"/>
-    <hyperlink ref="II7" r:id="rId164"/>
-    <hyperlink ref="IL7" r:id="rId165"/>
-    <hyperlink ref="IM7" r:id="rId166"/>
-    <hyperlink ref="L8" r:id="rId167"/>
-    <hyperlink ref="Q8" r:id="rId168"/>
-    <hyperlink ref="R8" r:id="rId169"/>
-    <hyperlink ref="V8" r:id="rId170"/>
-    <hyperlink ref="W8" r:id="rId171"/>
-    <hyperlink ref="AF8" r:id="rId172"/>
-    <hyperlink ref="AK8" r:id="rId173"/>
-    <hyperlink ref="AL8" r:id="rId174"/>
-    <hyperlink ref="AP8" r:id="rId175"/>
-    <hyperlink ref="AU8" r:id="rId176"/>
-    <hyperlink ref="AV8" r:id="rId177"/>
-    <hyperlink ref="AZ8" r:id="rId178"/>
-    <hyperlink ref="BE8" r:id="rId179"/>
-    <hyperlink ref="BF8" r:id="rId180"/>
-    <hyperlink ref="BP8" r:id="rId181"/>
-    <hyperlink ref="CC8" r:id="rId182"/>
-    <hyperlink ref="CD8" r:id="rId183"/>
-    <hyperlink ref="CH8" r:id="rId184"/>
-    <hyperlink ref="CI8" r:id="rId185"/>
-    <hyperlink ref="CL8" r:id="rId186"/>
-    <hyperlink ref="CM8" r:id="rId187"/>
-    <hyperlink ref="DU8" r:id="rId188"/>
-    <hyperlink ref="DY8" r:id="rId189"/>
-    <hyperlink ref="DZ8" r:id="rId190"/>
-    <hyperlink ref="EE8" r:id="rId191"/>
-    <hyperlink ref="FN8" r:id="rId192"/>
-    <hyperlink ref="HP8" r:id="rId193"/>
-    <hyperlink ref="HS8" r:id="rId194"/>
-    <hyperlink ref="HY8" r:id="rId195"/>
-    <hyperlink ref="HZ8" r:id="rId196"/>
-    <hyperlink ref="IH8" r:id="rId197"/>
-    <hyperlink ref="II8" r:id="rId198"/>
-    <hyperlink ref="IL8" r:id="rId199"/>
-    <hyperlink ref="IM8" r:id="rId200"/>
-    <hyperlink ref="L9" r:id="rId201"/>
-    <hyperlink ref="Q9" r:id="rId202"/>
-    <hyperlink ref="R9" r:id="rId203"/>
-    <hyperlink ref="V9" r:id="rId204"/>
-    <hyperlink ref="W9" r:id="rId205"/>
-    <hyperlink ref="AF9" r:id="rId206"/>
-    <hyperlink ref="AK9" r:id="rId207"/>
-    <hyperlink ref="AL9" r:id="rId208"/>
-    <hyperlink ref="AP9" r:id="rId209"/>
-    <hyperlink ref="AU9" r:id="rId210"/>
-    <hyperlink ref="AV9" r:id="rId211"/>
-    <hyperlink ref="AZ9" r:id="rId212"/>
-    <hyperlink ref="BE9" r:id="rId213"/>
-    <hyperlink ref="BF9" r:id="rId214"/>
-    <hyperlink ref="BP9" r:id="rId215"/>
-    <hyperlink ref="CC9" r:id="rId216"/>
-    <hyperlink ref="CD9" r:id="rId217"/>
-    <hyperlink ref="CH9" r:id="rId218"/>
-    <hyperlink ref="CI9" r:id="rId219"/>
-    <hyperlink ref="CL9" r:id="rId220"/>
-    <hyperlink ref="CM9" r:id="rId221"/>
-    <hyperlink ref="DU9" r:id="rId222"/>
-    <hyperlink ref="DZ9" r:id="rId223"/>
-    <hyperlink ref="ER9" r:id="rId224"/>
-    <hyperlink ref="HP9" r:id="rId225"/>
-    <hyperlink ref="HS9" r:id="rId226"/>
-    <hyperlink ref="HY9" r:id="rId227"/>
-    <hyperlink ref="HZ9" r:id="rId228"/>
-    <hyperlink ref="IH9" r:id="rId229"/>
-    <hyperlink ref="II9" r:id="rId230"/>
-    <hyperlink ref="IL9" r:id="rId231"/>
-    <hyperlink ref="IM9" r:id="rId232"/>
-    <hyperlink ref="L10" r:id="rId233"/>
-    <hyperlink ref="Q10" r:id="rId234"/>
-    <hyperlink ref="R10" r:id="rId235"/>
-    <hyperlink ref="V10" r:id="rId236"/>
-    <hyperlink ref="W10" r:id="rId237"/>
-    <hyperlink ref="AF10" r:id="rId238"/>
-    <hyperlink ref="AK10" r:id="rId239"/>
-    <hyperlink ref="AL10" r:id="rId240"/>
-    <hyperlink ref="AP10" r:id="rId241"/>
-    <hyperlink ref="AU10" r:id="rId242"/>
-    <hyperlink ref="AV10" r:id="rId243"/>
-    <hyperlink ref="AZ10" r:id="rId244"/>
-    <hyperlink ref="BE10" r:id="rId245"/>
-    <hyperlink ref="BF10" r:id="rId246"/>
-    <hyperlink ref="BP10" r:id="rId247"/>
-    <hyperlink ref="CC10" r:id="rId248"/>
-    <hyperlink ref="CD10" r:id="rId249"/>
-    <hyperlink ref="CH10" r:id="rId250"/>
-    <hyperlink ref="CI10" r:id="rId251"/>
-    <hyperlink ref="CL10" r:id="rId252"/>
-    <hyperlink ref="CM10" r:id="rId253"/>
-    <hyperlink ref="DU10" r:id="rId254"/>
-    <hyperlink ref="DY10" r:id="rId255"/>
-    <hyperlink ref="DZ10" r:id="rId256"/>
-    <hyperlink ref="EE10" r:id="rId257"/>
-    <hyperlink ref="ER10" r:id="rId258"/>
-    <hyperlink ref="FN10" r:id="rId259"/>
-    <hyperlink ref="FO10" r:id="rId260"/>
-    <hyperlink ref="HP10" r:id="rId261"/>
-    <hyperlink ref="HS10" r:id="rId262"/>
-    <hyperlink ref="HY10" r:id="rId263"/>
-    <hyperlink ref="HZ10" r:id="rId264"/>
-    <hyperlink ref="IH10" r:id="rId265"/>
-    <hyperlink ref="II10" r:id="rId266"/>
-    <hyperlink ref="IL10" r:id="rId267"/>
-    <hyperlink ref="IM10" r:id="rId268"/>
-    <hyperlink ref="L11" r:id="rId269"/>
-    <hyperlink ref="Q11" r:id="rId270"/>
-    <hyperlink ref="R11" r:id="rId271"/>
-    <hyperlink ref="V11" r:id="rId272"/>
-    <hyperlink ref="W11" r:id="rId273"/>
-    <hyperlink ref="AF11" r:id="rId274"/>
-    <hyperlink ref="AK11" r:id="rId275"/>
-    <hyperlink ref="AL11" r:id="rId276"/>
-    <hyperlink ref="AP11" r:id="rId277"/>
-    <hyperlink ref="AU11" r:id="rId278"/>
-    <hyperlink ref="AV11" r:id="rId279"/>
-    <hyperlink ref="AZ11" r:id="rId280"/>
-    <hyperlink ref="BE11" r:id="rId281"/>
-    <hyperlink ref="BF11" r:id="rId282"/>
-    <hyperlink ref="BP11" r:id="rId283"/>
-    <hyperlink ref="CC11" r:id="rId284"/>
-    <hyperlink ref="CD11" r:id="rId285"/>
-    <hyperlink ref="CH11" r:id="rId286"/>
-    <hyperlink ref="CI11" r:id="rId287"/>
-    <hyperlink ref="CL11" r:id="rId288"/>
-    <hyperlink ref="CM11" r:id="rId289"/>
-    <hyperlink ref="DU11" r:id="rId290"/>
-    <hyperlink ref="DY11" r:id="rId291"/>
-    <hyperlink ref="DZ11" r:id="rId292"/>
-    <hyperlink ref="ER11" r:id="rId293"/>
-    <hyperlink ref="EV11" r:id="rId294"/>
-    <hyperlink ref="EW11" r:id="rId295"/>
-    <hyperlink ref="FB11" r:id="rId296"/>
-    <hyperlink ref="GG11" r:id="rId297"/>
-    <hyperlink ref="GX11" r:id="rId298"/>
-    <hyperlink ref="GY11" r:id="rId299"/>
-    <hyperlink ref="HP11" r:id="rId300"/>
-    <hyperlink ref="HS11" r:id="rId301"/>
-    <hyperlink ref="HY11" r:id="rId302"/>
-    <hyperlink ref="HZ11" r:id="rId303"/>
-    <hyperlink ref="IH11" r:id="rId304"/>
-    <hyperlink ref="II11" r:id="rId305"/>
-    <hyperlink ref="IL11" r:id="rId306"/>
-    <hyperlink ref="IM11" r:id="rId307"/>
-    <hyperlink ref="L12" r:id="rId308"/>
-    <hyperlink ref="Q12" r:id="rId309"/>
-    <hyperlink ref="R12" r:id="rId310"/>
-    <hyperlink ref="V12" r:id="rId311"/>
-    <hyperlink ref="W12" r:id="rId312"/>
-    <hyperlink ref="AF12" r:id="rId313"/>
-    <hyperlink ref="AK12" r:id="rId314"/>
-    <hyperlink ref="AL12" r:id="rId315"/>
-    <hyperlink ref="AP12" r:id="rId316"/>
-    <hyperlink ref="AU12" r:id="rId317"/>
-    <hyperlink ref="AV12" r:id="rId318"/>
-    <hyperlink ref="AZ12" r:id="rId319"/>
-    <hyperlink ref="BP12" r:id="rId320"/>
-    <hyperlink ref="CC12" r:id="rId321"/>
-    <hyperlink ref="CD12" r:id="rId322"/>
-    <hyperlink ref="CH12" r:id="rId323"/>
-    <hyperlink ref="CI12" r:id="rId324"/>
-    <hyperlink ref="CL12" r:id="rId325"/>
-    <hyperlink ref="CM12" r:id="rId326"/>
-    <hyperlink ref="DU12" r:id="rId327"/>
-    <hyperlink ref="DZ12" r:id="rId328"/>
-    <hyperlink ref="ER12" r:id="rId329"/>
-    <hyperlink ref="EV12" r:id="rId330"/>
-    <hyperlink ref="EW12" r:id="rId331"/>
-    <hyperlink ref="FB12" r:id="rId332"/>
-    <hyperlink ref="FO12" r:id="rId333"/>
-    <hyperlink ref="GG12" r:id="rId334"/>
-    <hyperlink ref="HP12" r:id="rId335"/>
-    <hyperlink ref="HS12" r:id="rId336"/>
-    <hyperlink ref="HY12" r:id="rId337"/>
-    <hyperlink ref="HZ12" r:id="rId338"/>
-    <hyperlink ref="IH12" r:id="rId339"/>
-    <hyperlink ref="II12" r:id="rId340"/>
-    <hyperlink ref="IL12" r:id="rId341"/>
-    <hyperlink ref="IM12" r:id="rId342"/>
-    <hyperlink ref="L13" r:id="rId343"/>
-    <hyperlink ref="Q13" r:id="rId344"/>
-    <hyperlink ref="R13" r:id="rId345"/>
-    <hyperlink ref="V13" r:id="rId346"/>
-    <hyperlink ref="W13" r:id="rId347"/>
-    <hyperlink ref="AF13" r:id="rId348"/>
-    <hyperlink ref="AK13" r:id="rId349"/>
-    <hyperlink ref="AL13" r:id="rId350"/>
-    <hyperlink ref="AP13" r:id="rId351"/>
-    <hyperlink ref="AU13" r:id="rId352"/>
-    <hyperlink ref="AV13" r:id="rId353"/>
-    <hyperlink ref="AZ13" r:id="rId354"/>
-    <hyperlink ref="BE13" r:id="rId355"/>
-    <hyperlink ref="BF13" r:id="rId356"/>
-    <hyperlink ref="BP13" r:id="rId357"/>
-    <hyperlink ref="CC13" r:id="rId358"/>
-    <hyperlink ref="CD13" r:id="rId359"/>
-    <hyperlink ref="CH13" r:id="rId360"/>
-    <hyperlink ref="CI13" r:id="rId361"/>
-    <hyperlink ref="CL13" r:id="rId362"/>
-    <hyperlink ref="CM13" r:id="rId363"/>
-    <hyperlink ref="DU13" r:id="rId364"/>
-    <hyperlink ref="DY13" r:id="rId365"/>
-    <hyperlink ref="DZ13" r:id="rId366"/>
-    <hyperlink ref="HP13" r:id="rId367"/>
-    <hyperlink ref="HS13" r:id="rId368"/>
-    <hyperlink ref="HY13" r:id="rId369"/>
-    <hyperlink ref="HZ13" r:id="rId370"/>
-    <hyperlink ref="IH13" r:id="rId371"/>
-    <hyperlink ref="II13" r:id="rId372"/>
-    <hyperlink ref="IL13" r:id="rId373"/>
-    <hyperlink ref="IM13" r:id="rId374"/>
-    <hyperlink ref="L14" r:id="rId375"/>
-    <hyperlink ref="Q14" r:id="rId376"/>
-    <hyperlink ref="R14" r:id="rId377"/>
-    <hyperlink ref="V14" r:id="rId378"/>
-    <hyperlink ref="W14" r:id="rId379"/>
-    <hyperlink ref="AF14" r:id="rId380"/>
-    <hyperlink ref="AK14" r:id="rId381"/>
-    <hyperlink ref="AL14" r:id="rId382"/>
-    <hyperlink ref="AP14" r:id="rId383"/>
-    <hyperlink ref="AU14" r:id="rId384"/>
-    <hyperlink ref="AV14" r:id="rId385"/>
-    <hyperlink ref="AZ14" r:id="rId386"/>
-    <hyperlink ref="BE14" r:id="rId387"/>
-    <hyperlink ref="BF14" r:id="rId388"/>
-    <hyperlink ref="BP14" r:id="rId389"/>
-    <hyperlink ref="CC14" r:id="rId390"/>
-    <hyperlink ref="CD14" r:id="rId391"/>
-    <hyperlink ref="CH14" r:id="rId392"/>
-    <hyperlink ref="CI14" r:id="rId393"/>
-    <hyperlink ref="CL14" r:id="rId394"/>
-    <hyperlink ref="CM14" r:id="rId395"/>
-    <hyperlink ref="DU14" r:id="rId396"/>
-    <hyperlink ref="HP14" r:id="rId397"/>
-    <hyperlink ref="HS14" r:id="rId398"/>
-    <hyperlink ref="HY14" r:id="rId399"/>
-    <hyperlink ref="HZ14" r:id="rId400"/>
-    <hyperlink ref="IH14" r:id="rId401"/>
-    <hyperlink ref="II14" r:id="rId402"/>
-    <hyperlink ref="IL14" r:id="rId403"/>
-    <hyperlink ref="IM14" r:id="rId404"/>
-    <hyperlink ref="L15" r:id="rId405"/>
-    <hyperlink ref="Q15" r:id="rId406"/>
-    <hyperlink ref="R15" r:id="rId407"/>
-    <hyperlink ref="V15" r:id="rId408"/>
-    <hyperlink ref="W15" r:id="rId409"/>
-    <hyperlink ref="AA15" r:id="rId410"/>
-    <hyperlink ref="AB15" r:id="rId411"/>
-    <hyperlink ref="AF15" r:id="rId412"/>
-    <hyperlink ref="AK15" r:id="rId413"/>
-    <hyperlink ref="AL15" r:id="rId414"/>
-    <hyperlink ref="AP15" r:id="rId415"/>
-    <hyperlink ref="AU15" r:id="rId416"/>
-    <hyperlink ref="AV15" r:id="rId417"/>
-    <hyperlink ref="AZ15" r:id="rId418"/>
-    <hyperlink ref="BE15" r:id="rId419"/>
-    <hyperlink ref="BF15" r:id="rId420"/>
-    <hyperlink ref="BP15" r:id="rId421"/>
-    <hyperlink ref="CC15" r:id="rId422"/>
-    <hyperlink ref="CD15" r:id="rId423"/>
-    <hyperlink ref="CH15" r:id="rId424"/>
-    <hyperlink ref="CI15" r:id="rId425"/>
-    <hyperlink ref="CL15" r:id="rId426"/>
-    <hyperlink ref="CM15" r:id="rId427"/>
-    <hyperlink ref="DU15" r:id="rId428"/>
-    <hyperlink ref="DY15" r:id="rId429"/>
-    <hyperlink ref="DZ15" r:id="rId430"/>
-    <hyperlink ref="EE15" r:id="rId431"/>
-    <hyperlink ref="ER15" r:id="rId432"/>
-    <hyperlink ref="EV15" r:id="rId433"/>
-    <hyperlink ref="EW15" r:id="rId434"/>
-    <hyperlink ref="FB15" r:id="rId435"/>
-    <hyperlink ref="FO15" r:id="rId436"/>
-    <hyperlink ref="GG15" r:id="rId437"/>
-    <hyperlink ref="HP15" r:id="rId438"/>
-    <hyperlink ref="HS15" r:id="rId439"/>
-    <hyperlink ref="HY15" r:id="rId440"/>
-    <hyperlink ref="HZ15" r:id="rId441"/>
-    <hyperlink ref="IH15" r:id="rId442"/>
-    <hyperlink ref="II15" r:id="rId443"/>
-    <hyperlink ref="IL15" r:id="rId444"/>
-    <hyperlink ref="IM15" r:id="rId445"/>
-    <hyperlink ref="L16" r:id="rId446"/>
-    <hyperlink ref="Q16" r:id="rId447"/>
-    <hyperlink ref="R16" r:id="rId448"/>
-    <hyperlink ref="V16" r:id="rId449"/>
-    <hyperlink ref="W16" r:id="rId450"/>
-    <hyperlink ref="AF16" r:id="rId451"/>
-    <hyperlink ref="AK16" r:id="rId452"/>
-    <hyperlink ref="AL16" r:id="rId453"/>
-    <hyperlink ref="AP16" r:id="rId454"/>
-    <hyperlink ref="AU16" r:id="rId455"/>
-    <hyperlink ref="AV16" r:id="rId456"/>
-    <hyperlink ref="AZ16" r:id="rId457"/>
-    <hyperlink ref="BE16" r:id="rId458"/>
-    <hyperlink ref="BF16" r:id="rId459"/>
-    <hyperlink ref="BP16" r:id="rId460"/>
-    <hyperlink ref="CC16" r:id="rId461"/>
-    <hyperlink ref="CD16" r:id="rId462"/>
-    <hyperlink ref="CH16" r:id="rId463"/>
-    <hyperlink ref="CI16" r:id="rId464"/>
-    <hyperlink ref="CL16" r:id="rId465"/>
-    <hyperlink ref="CM16" r:id="rId466"/>
-    <hyperlink ref="DU16" r:id="rId467"/>
-    <hyperlink ref="DY16" r:id="rId468"/>
-    <hyperlink ref="DZ16" r:id="rId469"/>
-    <hyperlink ref="EE16" r:id="rId470"/>
-    <hyperlink ref="ER16" r:id="rId471"/>
-    <hyperlink ref="EV16" r:id="rId472"/>
-    <hyperlink ref="EW16" r:id="rId473"/>
-    <hyperlink ref="FB16" r:id="rId474"/>
-    <hyperlink ref="FO16" r:id="rId475"/>
-    <hyperlink ref="GG16" r:id="rId476"/>
-    <hyperlink ref="HP16" r:id="rId477"/>
-    <hyperlink ref="HS16" r:id="rId478"/>
-    <hyperlink ref="HY16" r:id="rId479"/>
-    <hyperlink ref="HZ16" r:id="rId480"/>
-    <hyperlink ref="IH16" r:id="rId481"/>
-    <hyperlink ref="II16" r:id="rId482"/>
-    <hyperlink ref="IL16" r:id="rId483"/>
-    <hyperlink ref="IM16" r:id="rId484"/>
-    <hyperlink ref="L17" r:id="rId485"/>
-    <hyperlink ref="Q17" r:id="rId486"/>
-    <hyperlink ref="R17" r:id="rId487"/>
-    <hyperlink ref="V17" r:id="rId488"/>
-    <hyperlink ref="W17" r:id="rId489"/>
-    <hyperlink ref="AF17" r:id="rId490"/>
-    <hyperlink ref="AK17" r:id="rId491"/>
-    <hyperlink ref="AL17" r:id="rId492"/>
-    <hyperlink ref="AP17" r:id="rId493"/>
-    <hyperlink ref="AU17" r:id="rId494"/>
-    <hyperlink ref="AV17" r:id="rId495"/>
-    <hyperlink ref="AZ17" r:id="rId496"/>
-    <hyperlink ref="BE17" r:id="rId497"/>
-    <hyperlink ref="BF17" r:id="rId498"/>
-    <hyperlink ref="BP17" r:id="rId499"/>
-    <hyperlink ref="CC17" r:id="rId500"/>
-    <hyperlink ref="CD17" r:id="rId501"/>
-    <hyperlink ref="CH17" r:id="rId502"/>
-    <hyperlink ref="CI17" r:id="rId503"/>
-    <hyperlink ref="CL17" r:id="rId504"/>
-    <hyperlink ref="CM17" r:id="rId505"/>
-    <hyperlink ref="DU17" r:id="rId506"/>
-    <hyperlink ref="DY17" r:id="rId507"/>
-    <hyperlink ref="DZ17" r:id="rId508"/>
-    <hyperlink ref="EE17" r:id="rId509"/>
-    <hyperlink ref="FN17" r:id="rId510"/>
-    <hyperlink ref="HP17" r:id="rId511"/>
-    <hyperlink ref="HS17" r:id="rId512"/>
-    <hyperlink ref="HY17" r:id="rId513"/>
-    <hyperlink ref="HZ17" r:id="rId514"/>
-    <hyperlink ref="IH17" r:id="rId515"/>
-    <hyperlink ref="II17" r:id="rId516"/>
-    <hyperlink ref="IL17" r:id="rId517"/>
-    <hyperlink ref="IM17" r:id="rId518"/>
+    <hyperlink ref="CL4" r:id="rId45"/>
+    <hyperlink ref="CM4" r:id="rId46"/>
+    <hyperlink ref="DY4" r:id="rId47"/>
+    <hyperlink ref="DZ4" r:id="rId48"/>
+    <hyperlink ref="EE4" r:id="rId49"/>
+    <hyperlink ref="ER4" r:id="rId50"/>
+    <hyperlink ref="FO4" r:id="rId51"/>
+    <hyperlink ref="GF4" r:id="rId52"/>
+    <hyperlink ref="GG4" r:id="rId53"/>
+    <hyperlink ref="HP4" r:id="rId54"/>
+    <hyperlink ref="HS4" r:id="rId55"/>
+    <hyperlink ref="HY4" r:id="rId56"/>
+    <hyperlink ref="HZ4" r:id="rId57"/>
+    <hyperlink ref="IH4" r:id="rId58"/>
+    <hyperlink ref="II4" r:id="rId59"/>
+    <hyperlink ref="IL4" r:id="rId60"/>
+    <hyperlink ref="IM4" r:id="rId61"/>
+    <hyperlink ref="L5" r:id="rId62"/>
+    <hyperlink ref="Q5" r:id="rId63"/>
+    <hyperlink ref="R5" r:id="rId64"/>
+    <hyperlink ref="V5" r:id="rId65"/>
+    <hyperlink ref="W5" r:id="rId66"/>
+    <hyperlink ref="AF5" r:id="rId67"/>
+    <hyperlink ref="AK5" r:id="rId68"/>
+    <hyperlink ref="AL5" r:id="rId69"/>
+    <hyperlink ref="AP5" r:id="rId70"/>
+    <hyperlink ref="AU5" r:id="rId71"/>
+    <hyperlink ref="AV5" r:id="rId72"/>
+    <hyperlink ref="AZ5" r:id="rId73"/>
+    <hyperlink ref="BE5" r:id="rId74"/>
+    <hyperlink ref="BF5" r:id="rId75"/>
+    <hyperlink ref="BP5" r:id="rId76"/>
+    <hyperlink ref="CC5" r:id="rId77"/>
+    <hyperlink ref="CD5" r:id="rId78"/>
+    <hyperlink ref="CL5" r:id="rId79"/>
+    <hyperlink ref="CM5" r:id="rId80"/>
+    <hyperlink ref="DU5" r:id="rId81"/>
+    <hyperlink ref="EQ5" r:id="rId82"/>
+    <hyperlink ref="ER5" r:id="rId83"/>
+    <hyperlink ref="HP5" r:id="rId84"/>
+    <hyperlink ref="HS5" r:id="rId85"/>
+    <hyperlink ref="HY5" r:id="rId86"/>
+    <hyperlink ref="HZ5" r:id="rId87"/>
+    <hyperlink ref="IH5" r:id="rId88"/>
+    <hyperlink ref="II5" r:id="rId89"/>
+    <hyperlink ref="IL5" r:id="rId90"/>
+    <hyperlink ref="IM5" r:id="rId91"/>
+    <hyperlink ref="L6" r:id="rId92"/>
+    <hyperlink ref="Q6" r:id="rId93"/>
+    <hyperlink ref="R6" r:id="rId94"/>
+    <hyperlink ref="V6" r:id="rId95"/>
+    <hyperlink ref="W6" r:id="rId96"/>
+    <hyperlink ref="AA6" r:id="rId97"/>
+    <hyperlink ref="AB6" r:id="rId98"/>
+    <hyperlink ref="AF6" r:id="rId99"/>
+    <hyperlink ref="AK6" r:id="rId100"/>
+    <hyperlink ref="AL6" r:id="rId101"/>
+    <hyperlink ref="AP6" r:id="rId102"/>
+    <hyperlink ref="AU6" r:id="rId103"/>
+    <hyperlink ref="AV6" r:id="rId104"/>
+    <hyperlink ref="AZ6" r:id="rId105"/>
+    <hyperlink ref="BE6" r:id="rId106"/>
+    <hyperlink ref="BF6" r:id="rId107"/>
+    <hyperlink ref="BP6" r:id="rId108"/>
+    <hyperlink ref="CC6" r:id="rId109"/>
+    <hyperlink ref="CD6" r:id="rId110"/>
+    <hyperlink ref="CL6" r:id="rId111"/>
+    <hyperlink ref="CM6" r:id="rId112"/>
+    <hyperlink ref="DY6" r:id="rId113"/>
+    <hyperlink ref="DZ6" r:id="rId114"/>
+    <hyperlink ref="EE6" r:id="rId115"/>
+    <hyperlink ref="ER6" r:id="rId116"/>
+    <hyperlink ref="HP6" r:id="rId117"/>
+    <hyperlink ref="HS6" r:id="rId118"/>
+    <hyperlink ref="HY6" r:id="rId119"/>
+    <hyperlink ref="HZ6" r:id="rId120"/>
+    <hyperlink ref="IH6" r:id="rId121"/>
+    <hyperlink ref="II6" r:id="rId122"/>
+    <hyperlink ref="IL6" r:id="rId123"/>
+    <hyperlink ref="IM6" r:id="rId124"/>
+    <hyperlink ref="L7" r:id="rId125"/>
+    <hyperlink ref="Q7" r:id="rId126"/>
+    <hyperlink ref="R7" r:id="rId127"/>
+    <hyperlink ref="V7" r:id="rId128"/>
+    <hyperlink ref="W7" r:id="rId129"/>
+    <hyperlink ref="AF7" r:id="rId130"/>
+    <hyperlink ref="AK7" r:id="rId131"/>
+    <hyperlink ref="AL7" r:id="rId132"/>
+    <hyperlink ref="AP7" r:id="rId133"/>
+    <hyperlink ref="AU7" r:id="rId134"/>
+    <hyperlink ref="AV7" r:id="rId135"/>
+    <hyperlink ref="AZ7" r:id="rId136"/>
+    <hyperlink ref="BP7" r:id="rId137"/>
+    <hyperlink ref="CC7" r:id="rId138"/>
+    <hyperlink ref="CD7" r:id="rId139"/>
+    <hyperlink ref="CL7" r:id="rId140"/>
+    <hyperlink ref="CM7" r:id="rId141"/>
+    <hyperlink ref="DT7" r:id="rId142"/>
+    <hyperlink ref="DU7" r:id="rId143"/>
+    <hyperlink ref="ER7" r:id="rId144"/>
+    <hyperlink ref="FO7" r:id="rId145"/>
+    <hyperlink ref="FT7" r:id="rId146"/>
+    <hyperlink ref="GG7" r:id="rId147"/>
+    <hyperlink ref="GL7" r:id="rId148"/>
+    <hyperlink ref="GY7" r:id="rId149"/>
+    <hyperlink ref="HD7" r:id="rId150"/>
+    <hyperlink ref="HP7" r:id="rId151"/>
+    <hyperlink ref="HS7" r:id="rId152"/>
+    <hyperlink ref="HY7" r:id="rId153"/>
+    <hyperlink ref="HZ7" r:id="rId154"/>
+    <hyperlink ref="IH7" r:id="rId155"/>
+    <hyperlink ref="II7" r:id="rId156"/>
+    <hyperlink ref="IL7" r:id="rId157"/>
+    <hyperlink ref="IM7" r:id="rId158"/>
+    <hyperlink ref="L8" r:id="rId159"/>
+    <hyperlink ref="Q8" r:id="rId160"/>
+    <hyperlink ref="R8" r:id="rId161"/>
+    <hyperlink ref="V8" r:id="rId162"/>
+    <hyperlink ref="W8" r:id="rId163"/>
+    <hyperlink ref="AF8" r:id="rId164"/>
+    <hyperlink ref="AK8" r:id="rId165"/>
+    <hyperlink ref="AL8" r:id="rId166"/>
+    <hyperlink ref="AP8" r:id="rId167"/>
+    <hyperlink ref="AU8" r:id="rId168"/>
+    <hyperlink ref="AV8" r:id="rId169"/>
+    <hyperlink ref="AZ8" r:id="rId170"/>
+    <hyperlink ref="BE8" r:id="rId171"/>
+    <hyperlink ref="BF8" r:id="rId172"/>
+    <hyperlink ref="BP8" r:id="rId173"/>
+    <hyperlink ref="CC8" r:id="rId174"/>
+    <hyperlink ref="CD8" r:id="rId175"/>
+    <hyperlink ref="CL8" r:id="rId176"/>
+    <hyperlink ref="CM8" r:id="rId177"/>
+    <hyperlink ref="DU8" r:id="rId178"/>
+    <hyperlink ref="DY8" r:id="rId179"/>
+    <hyperlink ref="DZ8" r:id="rId180"/>
+    <hyperlink ref="EE8" r:id="rId181"/>
+    <hyperlink ref="FN8" r:id="rId182"/>
+    <hyperlink ref="HP8" r:id="rId183"/>
+    <hyperlink ref="HS8" r:id="rId184"/>
+    <hyperlink ref="HY8" r:id="rId185"/>
+    <hyperlink ref="HZ8" r:id="rId186"/>
+    <hyperlink ref="IH8" r:id="rId187"/>
+    <hyperlink ref="II8" r:id="rId188"/>
+    <hyperlink ref="IL8" r:id="rId189"/>
+    <hyperlink ref="IM8" r:id="rId190"/>
+    <hyperlink ref="L9" r:id="rId191"/>
+    <hyperlink ref="Q9" r:id="rId192"/>
+    <hyperlink ref="R9" r:id="rId193"/>
+    <hyperlink ref="V9" r:id="rId194"/>
+    <hyperlink ref="W9" r:id="rId195"/>
+    <hyperlink ref="AF9" r:id="rId196"/>
+    <hyperlink ref="AK9" r:id="rId197"/>
+    <hyperlink ref="AL9" r:id="rId198"/>
+    <hyperlink ref="AP9" r:id="rId199"/>
+    <hyperlink ref="AU9" r:id="rId200"/>
+    <hyperlink ref="AV9" r:id="rId201"/>
+    <hyperlink ref="AZ9" r:id="rId202"/>
+    <hyperlink ref="BE9" r:id="rId203"/>
+    <hyperlink ref="BF9" r:id="rId204"/>
+    <hyperlink ref="BP9" r:id="rId205"/>
+    <hyperlink ref="CC9" r:id="rId206"/>
+    <hyperlink ref="CD9" r:id="rId207"/>
+    <hyperlink ref="CL9" r:id="rId208"/>
+    <hyperlink ref="CM9" r:id="rId209"/>
+    <hyperlink ref="DU9" r:id="rId210"/>
+    <hyperlink ref="DZ9" r:id="rId211"/>
+    <hyperlink ref="ER9" r:id="rId212"/>
+    <hyperlink ref="HP9" r:id="rId213"/>
+    <hyperlink ref="HS9" r:id="rId214"/>
+    <hyperlink ref="HY9" r:id="rId215"/>
+    <hyperlink ref="HZ9" r:id="rId216"/>
+    <hyperlink ref="IH9" r:id="rId217"/>
+    <hyperlink ref="II9" r:id="rId218"/>
+    <hyperlink ref="IL9" r:id="rId219"/>
+    <hyperlink ref="IM9" r:id="rId220"/>
+    <hyperlink ref="L10" r:id="rId221"/>
+    <hyperlink ref="Q10" r:id="rId222"/>
+    <hyperlink ref="R10" r:id="rId223"/>
+    <hyperlink ref="V10" r:id="rId224"/>
+    <hyperlink ref="W10" r:id="rId225"/>
+    <hyperlink ref="AF10" r:id="rId226"/>
+    <hyperlink ref="AK10" r:id="rId227"/>
+    <hyperlink ref="AL10" r:id="rId228"/>
+    <hyperlink ref="AP10" r:id="rId229"/>
+    <hyperlink ref="AU10" r:id="rId230"/>
+    <hyperlink ref="AV10" r:id="rId231"/>
+    <hyperlink ref="AZ10" r:id="rId232"/>
+    <hyperlink ref="BE10" r:id="rId233"/>
+    <hyperlink ref="BF10" r:id="rId234"/>
+    <hyperlink ref="BP10" r:id="rId235"/>
+    <hyperlink ref="CC10" r:id="rId236"/>
+    <hyperlink ref="CD10" r:id="rId237"/>
+    <hyperlink ref="CL10" r:id="rId238"/>
+    <hyperlink ref="CM10" r:id="rId239"/>
+    <hyperlink ref="DU10" r:id="rId240"/>
+    <hyperlink ref="DY10" r:id="rId241"/>
+    <hyperlink ref="DZ10" r:id="rId242"/>
+    <hyperlink ref="EE10" r:id="rId243"/>
+    <hyperlink ref="ER10" r:id="rId244"/>
+    <hyperlink ref="FN10" r:id="rId245"/>
+    <hyperlink ref="FO10" r:id="rId246"/>
+    <hyperlink ref="HP10" r:id="rId247"/>
+    <hyperlink ref="HS10" r:id="rId248"/>
+    <hyperlink ref="HY10" r:id="rId249"/>
+    <hyperlink ref="HZ10" r:id="rId250"/>
+    <hyperlink ref="IH10" r:id="rId251"/>
+    <hyperlink ref="II10" r:id="rId252"/>
+    <hyperlink ref="IL10" r:id="rId253"/>
+    <hyperlink ref="IM10" r:id="rId254"/>
+    <hyperlink ref="L11" r:id="rId255"/>
+    <hyperlink ref="Q11" r:id="rId256"/>
+    <hyperlink ref="R11" r:id="rId257"/>
+    <hyperlink ref="V11" r:id="rId258"/>
+    <hyperlink ref="W11" r:id="rId259"/>
+    <hyperlink ref="AF11" r:id="rId260"/>
+    <hyperlink ref="AK11" r:id="rId261"/>
+    <hyperlink ref="AL11" r:id="rId262"/>
+    <hyperlink ref="AP11" r:id="rId263"/>
+    <hyperlink ref="AU11" r:id="rId264"/>
+    <hyperlink ref="AV11" r:id="rId265"/>
+    <hyperlink ref="AZ11" r:id="rId266"/>
+    <hyperlink ref="BE11" r:id="rId267"/>
+    <hyperlink ref="BF11" r:id="rId268"/>
+    <hyperlink ref="BP11" r:id="rId269"/>
+    <hyperlink ref="CC11" r:id="rId270"/>
+    <hyperlink ref="CD11" r:id="rId271"/>
+    <hyperlink ref="CL11" r:id="rId272"/>
+    <hyperlink ref="CM11" r:id="rId273"/>
+    <hyperlink ref="DU11" r:id="rId274"/>
+    <hyperlink ref="DY11" r:id="rId275"/>
+    <hyperlink ref="DZ11" r:id="rId276"/>
+    <hyperlink ref="ER11" r:id="rId277"/>
+    <hyperlink ref="EV11" r:id="rId278"/>
+    <hyperlink ref="EW11" r:id="rId279"/>
+    <hyperlink ref="FB11" r:id="rId280"/>
+    <hyperlink ref="GG11" r:id="rId281"/>
+    <hyperlink ref="GX11" r:id="rId282"/>
+    <hyperlink ref="GY11" r:id="rId283"/>
+    <hyperlink ref="HP11" r:id="rId284"/>
+    <hyperlink ref="HS11" r:id="rId285"/>
+    <hyperlink ref="HY11" r:id="rId286"/>
+    <hyperlink ref="HZ11" r:id="rId287"/>
+    <hyperlink ref="IH11" r:id="rId288"/>
+    <hyperlink ref="II11" r:id="rId289"/>
+    <hyperlink ref="IL11" r:id="rId290"/>
+    <hyperlink ref="IM11" r:id="rId291"/>
+    <hyperlink ref="L12" r:id="rId292"/>
+    <hyperlink ref="Q12" r:id="rId293"/>
+    <hyperlink ref="R12" r:id="rId294"/>
+    <hyperlink ref="V12" r:id="rId295"/>
+    <hyperlink ref="W12" r:id="rId296"/>
+    <hyperlink ref="AF12" r:id="rId297"/>
+    <hyperlink ref="AK12" r:id="rId298"/>
+    <hyperlink ref="AL12" r:id="rId299"/>
+    <hyperlink ref="AP12" r:id="rId300"/>
+    <hyperlink ref="AU12" r:id="rId301"/>
+    <hyperlink ref="AV12" r:id="rId302"/>
+    <hyperlink ref="AZ12" r:id="rId303"/>
+    <hyperlink ref="BP12" r:id="rId304"/>
+    <hyperlink ref="CC12" r:id="rId305"/>
+    <hyperlink ref="CD12" r:id="rId306"/>
+    <hyperlink ref="CL12" r:id="rId307"/>
+    <hyperlink ref="CM12" r:id="rId308"/>
+    <hyperlink ref="DU12" r:id="rId309"/>
+    <hyperlink ref="DZ12" r:id="rId310"/>
+    <hyperlink ref="ER12" r:id="rId311"/>
+    <hyperlink ref="EV12" r:id="rId312"/>
+    <hyperlink ref="EW12" r:id="rId313"/>
+    <hyperlink ref="FB12" r:id="rId314"/>
+    <hyperlink ref="FO12" r:id="rId315"/>
+    <hyperlink ref="GG12" r:id="rId316"/>
+    <hyperlink ref="HP12" r:id="rId317"/>
+    <hyperlink ref="HS12" r:id="rId318"/>
+    <hyperlink ref="HY12" r:id="rId319"/>
+    <hyperlink ref="HZ12" r:id="rId320"/>
+    <hyperlink ref="IH12" r:id="rId321"/>
+    <hyperlink ref="II12" r:id="rId322"/>
+    <hyperlink ref="IL12" r:id="rId323"/>
+    <hyperlink ref="IM12" r:id="rId324"/>
+    <hyperlink ref="L13" r:id="rId325"/>
+    <hyperlink ref="Q13" r:id="rId326"/>
+    <hyperlink ref="R13" r:id="rId327"/>
+    <hyperlink ref="V13" r:id="rId328"/>
+    <hyperlink ref="W13" r:id="rId329"/>
+    <hyperlink ref="AF13" r:id="rId330"/>
+    <hyperlink ref="AK13" r:id="rId331"/>
+    <hyperlink ref="AL13" r:id="rId332"/>
+    <hyperlink ref="AP13" r:id="rId333"/>
+    <hyperlink ref="AU13" r:id="rId334"/>
+    <hyperlink ref="AV13" r:id="rId335"/>
+    <hyperlink ref="AZ13" r:id="rId336"/>
+    <hyperlink ref="BE13" r:id="rId337"/>
+    <hyperlink ref="BF13" r:id="rId338"/>
+    <hyperlink ref="BP13" r:id="rId339"/>
+    <hyperlink ref="CC13" r:id="rId340"/>
+    <hyperlink ref="CD13" r:id="rId341"/>
+    <hyperlink ref="CL13" r:id="rId342"/>
+    <hyperlink ref="CM13" r:id="rId343"/>
+    <hyperlink ref="DU13" r:id="rId344"/>
+    <hyperlink ref="DY13" r:id="rId345"/>
+    <hyperlink ref="DZ13" r:id="rId346"/>
+    <hyperlink ref="HP13" r:id="rId347"/>
+    <hyperlink ref="HS13" r:id="rId348"/>
+    <hyperlink ref="HY13" r:id="rId349"/>
+    <hyperlink ref="HZ13" r:id="rId350"/>
+    <hyperlink ref="IH13" r:id="rId351"/>
+    <hyperlink ref="II13" r:id="rId352"/>
+    <hyperlink ref="IL13" r:id="rId353"/>
+    <hyperlink ref="IM13" r:id="rId354"/>
+    <hyperlink ref="L14" r:id="rId355"/>
+    <hyperlink ref="Q14" r:id="rId356"/>
+    <hyperlink ref="R14" r:id="rId357"/>
+    <hyperlink ref="V14" r:id="rId358"/>
+    <hyperlink ref="W14" r:id="rId359"/>
+    <hyperlink ref="AF14" r:id="rId360"/>
+    <hyperlink ref="AK14" r:id="rId361"/>
+    <hyperlink ref="AL14" r:id="rId362"/>
+    <hyperlink ref="AP14" r:id="rId363"/>
+    <hyperlink ref="AU14" r:id="rId364"/>
+    <hyperlink ref="AV14" r:id="rId365"/>
+    <hyperlink ref="AZ14" r:id="rId366"/>
+    <hyperlink ref="BE14" r:id="rId367"/>
+    <hyperlink ref="BF14" r:id="rId368"/>
+    <hyperlink ref="BP14" r:id="rId369"/>
+    <hyperlink ref="CC14" r:id="rId370"/>
+    <hyperlink ref="CD14" r:id="rId371"/>
+    <hyperlink ref="CL14" r:id="rId372"/>
+    <hyperlink ref="CM14" r:id="rId373"/>
+    <hyperlink ref="DU14" r:id="rId374"/>
+    <hyperlink ref="HP14" r:id="rId375"/>
+    <hyperlink ref="HS14" r:id="rId376"/>
+    <hyperlink ref="HY14" r:id="rId377"/>
+    <hyperlink ref="HZ14" r:id="rId378"/>
+    <hyperlink ref="IH14" r:id="rId379"/>
+    <hyperlink ref="II14" r:id="rId380"/>
+    <hyperlink ref="IL14" r:id="rId381"/>
+    <hyperlink ref="IM14" r:id="rId382"/>
+    <hyperlink ref="L15" r:id="rId383"/>
+    <hyperlink ref="Q15" r:id="rId384"/>
+    <hyperlink ref="R15" r:id="rId385"/>
+    <hyperlink ref="V15" r:id="rId386"/>
+    <hyperlink ref="W15" r:id="rId387"/>
+    <hyperlink ref="AA15" r:id="rId388"/>
+    <hyperlink ref="AB15" r:id="rId389"/>
+    <hyperlink ref="AF15" r:id="rId390"/>
+    <hyperlink ref="AK15" r:id="rId391"/>
+    <hyperlink ref="AL15" r:id="rId392"/>
+    <hyperlink ref="AP15" r:id="rId393"/>
+    <hyperlink ref="AU15" r:id="rId394"/>
+    <hyperlink ref="AV15" r:id="rId395"/>
+    <hyperlink ref="AZ15" r:id="rId396"/>
+    <hyperlink ref="BE15" r:id="rId397"/>
+    <hyperlink ref="BF15" r:id="rId398"/>
+    <hyperlink ref="BP15" r:id="rId399"/>
+    <hyperlink ref="CC15" r:id="rId400"/>
+    <hyperlink ref="CD15" r:id="rId401"/>
+    <hyperlink ref="CL15" r:id="rId402"/>
+    <hyperlink ref="CM15" r:id="rId403"/>
+    <hyperlink ref="DU15" r:id="rId404"/>
+    <hyperlink ref="DY15" r:id="rId405"/>
+    <hyperlink ref="DZ15" r:id="rId406"/>
+    <hyperlink ref="EE15" r:id="rId407"/>
+    <hyperlink ref="ER15" r:id="rId408"/>
+    <hyperlink ref="EV15" r:id="rId409"/>
+    <hyperlink ref="EW15" r:id="rId410"/>
+    <hyperlink ref="FB15" r:id="rId411"/>
+    <hyperlink ref="FO15" r:id="rId412"/>
+    <hyperlink ref="GG15" r:id="rId413"/>
+    <hyperlink ref="HP15" r:id="rId414"/>
+    <hyperlink ref="HS15" r:id="rId415"/>
+    <hyperlink ref="HY15" r:id="rId416"/>
+    <hyperlink ref="HZ15" r:id="rId417"/>
+    <hyperlink ref="IH15" r:id="rId418"/>
+    <hyperlink ref="II15" r:id="rId419"/>
+    <hyperlink ref="IL15" r:id="rId420"/>
+    <hyperlink ref="IM15" r:id="rId421"/>
+    <hyperlink ref="L16" r:id="rId422"/>
+    <hyperlink ref="Q16" r:id="rId423"/>
+    <hyperlink ref="R16" r:id="rId424"/>
+    <hyperlink ref="V16" r:id="rId425"/>
+    <hyperlink ref="W16" r:id="rId426"/>
+    <hyperlink ref="AF16" r:id="rId427"/>
+    <hyperlink ref="AK16" r:id="rId428"/>
+    <hyperlink ref="AL16" r:id="rId429"/>
+    <hyperlink ref="AP16" r:id="rId430"/>
+    <hyperlink ref="AU16" r:id="rId431"/>
+    <hyperlink ref="AV16" r:id="rId432"/>
+    <hyperlink ref="AZ16" r:id="rId433"/>
+    <hyperlink ref="BE16" r:id="rId434"/>
+    <hyperlink ref="BF16" r:id="rId435"/>
+    <hyperlink ref="BP16" r:id="rId436"/>
+    <hyperlink ref="CC16" r:id="rId437"/>
+    <hyperlink ref="CD16" r:id="rId438"/>
+    <hyperlink ref="CL16" r:id="rId439"/>
+    <hyperlink ref="CM16" r:id="rId440"/>
+    <hyperlink ref="DU16" r:id="rId441"/>
+    <hyperlink ref="DY16" r:id="rId442"/>
+    <hyperlink ref="DZ16" r:id="rId443"/>
+    <hyperlink ref="EE16" r:id="rId444"/>
+    <hyperlink ref="ER16" r:id="rId445"/>
+    <hyperlink ref="EV16" r:id="rId446"/>
+    <hyperlink ref="EW16" r:id="rId447"/>
+    <hyperlink ref="FB16" r:id="rId448"/>
+    <hyperlink ref="FO16" r:id="rId449"/>
+    <hyperlink ref="GG16" r:id="rId450"/>
+    <hyperlink ref="HP16" r:id="rId451"/>
+    <hyperlink ref="HS16" r:id="rId452"/>
+    <hyperlink ref="HY16" r:id="rId453"/>
+    <hyperlink ref="HZ16" r:id="rId454"/>
+    <hyperlink ref="IH16" r:id="rId455"/>
+    <hyperlink ref="II16" r:id="rId456"/>
+    <hyperlink ref="IL16" r:id="rId457"/>
+    <hyperlink ref="IM16" r:id="rId458"/>
+    <hyperlink ref="L17" r:id="rId459"/>
+    <hyperlink ref="Q17" r:id="rId460"/>
+    <hyperlink ref="R17" r:id="rId461"/>
+    <hyperlink ref="V17" r:id="rId462"/>
+    <hyperlink ref="W17" r:id="rId463"/>
+    <hyperlink ref="AF17" r:id="rId464"/>
+    <hyperlink ref="AK17" r:id="rId465"/>
+    <hyperlink ref="AL17" r:id="rId466"/>
+    <hyperlink ref="AP17" r:id="rId467"/>
+    <hyperlink ref="AU17" r:id="rId468"/>
+    <hyperlink ref="AV17" r:id="rId469"/>
+    <hyperlink ref="AZ17" r:id="rId470"/>
+    <hyperlink ref="BE17" r:id="rId471"/>
+    <hyperlink ref="BF17" r:id="rId472"/>
+    <hyperlink ref="BP17" r:id="rId473"/>
+    <hyperlink ref="CC17" r:id="rId474"/>
+    <hyperlink ref="CD17" r:id="rId475"/>
+    <hyperlink ref="CL17" r:id="rId476"/>
+    <hyperlink ref="CM17" r:id="rId477"/>
+    <hyperlink ref="DU17" r:id="rId478"/>
+    <hyperlink ref="DY17" r:id="rId479"/>
+    <hyperlink ref="DZ17" r:id="rId480"/>
+    <hyperlink ref="EE17" r:id="rId481"/>
+    <hyperlink ref="FN17" r:id="rId482"/>
+    <hyperlink ref="HP17" r:id="rId483"/>
+    <hyperlink ref="HS17" r:id="rId484"/>
+    <hyperlink ref="HY17" r:id="rId485"/>
+    <hyperlink ref="HZ17" r:id="rId486"/>
+    <hyperlink ref="IH17" r:id="rId487"/>
+    <hyperlink ref="II17" r:id="rId488"/>
+    <hyperlink ref="IL17" r:id="rId489"/>
+    <hyperlink ref="IM17" r:id="rId490"/>
+    <hyperlink ref="CH4" r:id="rId491" display="http://id.loc.gov/vocabulary/languages"/>
+    <hyperlink ref="CH5" r:id="rId492" display="http://id.loc.gov/vocabulary/languages"/>
+    <hyperlink ref="CH6" r:id="rId493" display="http://id.loc.gov/vocabulary/languages"/>
+    <hyperlink ref="CH7" r:id="rId494" display="http://id.loc.gov/vocabulary/languages"/>
+    <hyperlink ref="CH8" r:id="rId495" display="http://id.loc.gov/vocabulary/languages"/>
+    <hyperlink ref="CH9" r:id="rId496" display="http://id.loc.gov/vocabulary/languages"/>
+    <hyperlink ref="CH10" r:id="rId497" display="http://id.loc.gov/vocabulary/languages"/>
+    <hyperlink ref="CH11" r:id="rId498" display="http://id.loc.gov/vocabulary/languages"/>
+    <hyperlink ref="CH12" r:id="rId499" display="http://id.loc.gov/vocabulary/languages"/>
+    <hyperlink ref="CH13" r:id="rId500" display="http://id.loc.gov/vocabulary/languages"/>
+    <hyperlink ref="CH14" r:id="rId501" display="http://id.loc.gov/vocabulary/languages"/>
+    <hyperlink ref="CH15" r:id="rId502" display="http://id.loc.gov/vocabulary/languages"/>
+    <hyperlink ref="CH16" r:id="rId503" display="http://id.loc.gov/vocabulary/languages"/>
+    <hyperlink ref="CH17" r:id="rId504" display="http://id.loc.gov/vocabulary/languages"/>
+    <hyperlink ref="CI4" r:id="rId505" display="http://id.loc.gov/vocabulary/languages/eng"/>
+    <hyperlink ref="CI5" r:id="rId506" display="http://id.loc.gov/vocabulary/languages/eng"/>
+    <hyperlink ref="CI6" r:id="rId507" display="http://id.loc.gov/vocabulary/languages/eng"/>
+    <hyperlink ref="CI7" r:id="rId508" display="http://id.loc.gov/vocabulary/languages/eng"/>
+    <hyperlink ref="CI8" r:id="rId509" display="http://id.loc.gov/vocabulary/languages/eng"/>
+    <hyperlink ref="CI9" r:id="rId510" display="http://id.loc.gov/vocabulary/languages/eng"/>
+    <hyperlink ref="CI10" r:id="rId511" display="http://id.loc.gov/vocabulary/languages/eng"/>
+    <hyperlink ref="CI11" r:id="rId512" display="http://id.loc.gov/vocabulary/languages/eng"/>
+    <hyperlink ref="CI12" r:id="rId513" display="http://id.loc.gov/vocabulary/languages/eng"/>
+    <hyperlink ref="CI13" r:id="rId514" display="http://id.loc.gov/vocabulary/languages/eng"/>
+    <hyperlink ref="CI14" r:id="rId515" display="http://id.loc.gov/vocabulary/languages/eng"/>
+    <hyperlink ref="CI15" r:id="rId516" display="http://id.loc.gov/vocabulary/languages/eng"/>
+    <hyperlink ref="CI16" r:id="rId517" display="http://id.loc.gov/vocabulary/languages/eng"/>
+    <hyperlink ref="CI17" r:id="rId518" display="http://id.loc.gov/vocabulary/languages/eng"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId519"/>

</xml_diff>